<commit_message>
Add of the javaTypeForIDType (StarWars sample uses it)
</commit_message>
<xml_diff>
--- a/graphql-maven-plugin-samples/graphql-maven-plugin-samples-Forum-server/src/main/resources/data.xlsx
+++ b/graphql-maven-plugin-samples/graphql-maven-plugin-samples-Forum-server/src/main/resources/data.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7230ECAB-C513-4A62-896E-9581AC52D43A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="6" r:id="rId1"/>
@@ -15,7 +14,7 @@
     <sheet name="post" sheetId="4" r:id="rId5"/>
     <sheet name="agregated SQL" sheetId="5" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -291,9 +290,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -349,8 +348,8 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -359,10 +358,7 @@
   </cellStyles>
   <dxfs count="37">
     <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -404,44 +400,7 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -466,13 +425,27 @@
         <sz val="10"/>
         <color theme="1"/>
         <name val="Consolas"/>
-        <family val="3"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -497,13 +470,9 @@
         <sz val="10"/>
         <color theme="1"/>
         <name val="Consolas"/>
-        <family val="3"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -528,7 +497,33 @@
         <sz val="10"/>
         <color theme="1"/>
         <name val="Consolas"/>
-        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -547,25 +542,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0B2A3854-B99B-4181-86F1-DB4B56252B89}" name="Tableau1" displayName="Tableau1" ref="A1:G45" totalsRowShown="0" headerRowDxfId="36">
-  <autoFilter ref="A1:G45" xr:uid="{E51E0535-57DD-4C85-BD8D-85F8947315F0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:G45" totalsRowShown="0" headerRowDxfId="36">
+  <autoFilter ref="A1:G45"/>
   <tableColumns count="7">
-    <tableColumn id="7" xr3:uid="{8762674C-F6A9-499A-95CB-E30F8E49B464}" name="num ligne" dataDxfId="35">
+    <tableColumn id="7" name="num ligne" dataDxfId="35">
       <calculatedColumnFormula>ROW()-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{C454B158-4E2C-494C-BA65-332B0084ACBB}" name="id" dataDxfId="34">
+    <tableColumn id="1" name="id" dataDxfId="34">
       <calculatedColumnFormula>Tableau1[[#This Row],[num ligne]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{A359D3FB-13C3-4A33-8B6F-1126851C3BC6}" name="name"/>
-    <tableColumn id="3" xr3:uid="{D1DF648F-A878-4A1A-AFA9-50705FE02346}" name="alias">
+    <tableColumn id="2" name="name"/>
+    <tableColumn id="3" name="alias">
       <calculatedColumnFormula>IF(MOD(ROW(),2)=0,"null","Alias of "&amp;C2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{689CEC51-8C28-43CA-A450-FAE8CFA218B8}" name="email" dataDxfId="33">
+    <tableColumn id="4" name="email" dataDxfId="33">
       <calculatedColumnFormula>SUBSTITUTE(LOWER(C2), " ", ".") &amp; "@graphql-java.com"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{68033CB6-28E0-4C83-8FA5-957420F7B64F}" name="type"/>
-    <tableColumn id="6" xr3:uid="{5DBA6BC6-BA5E-45B6-9E43-9870D875E8F5}" name="SQL" dataDxfId="32">
-      <calculatedColumnFormula>"insert into member (id, name, alias, email, type) values ('"&amp;B2&amp;"', '"&amp;C2&amp;"', "&amp;IF(D2="null","null","'" &amp; D2 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</calculatedColumnFormula>
+    <tableColumn id="5" name="type"/>
+    <tableColumn id="6" name="SQL" dataDxfId="2">
+      <calculatedColumnFormula>"insert into member (id, name, alias, email, type) values ("&amp;B2&amp;", '"&amp;C2&amp;"', "&amp;IF(D2="null","null","'" &amp; D2 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -573,21 +568,21 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{12FB436E-4392-48E3-AA46-97405E326A83}" name="Tableau13" displayName="Tableau13" ref="A1:E11" totalsRowShown="0" headerRowDxfId="31">
-  <autoFilter ref="A1:E11" xr:uid="{8DEAF3DC-02AF-470F-8CA2-FE34E33F8A01}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau13" displayName="Tableau13" ref="A1:E11" totalsRowShown="0" headerRowDxfId="32">
+  <autoFilter ref="A1:E11"/>
   <tableColumns count="5">
-    <tableColumn id="7" xr3:uid="{BCC10D84-5811-46DC-AC01-B619481041CD}" name="num ligne" dataDxfId="30">
+    <tableColumn id="7" name="num ligne" dataDxfId="31">
       <calculatedColumnFormula>ROW()-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{DAE3285A-EAB7-45E4-A1A2-1839F671D573}" name="id" dataDxfId="29">
+    <tableColumn id="1" name="id" dataDxfId="30">
       <calculatedColumnFormula>Tableau13[[#This Row],[num ligne]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{C63CB093-510D-40A0-9990-89B48ED8B670}" name="name"/>
-    <tableColumn id="3" xr3:uid="{845CD4C0-0826-445B-9DF3-348404799731}" name="publiclyAvailable" dataDxfId="28">
+    <tableColumn id="2" name="name"/>
+    <tableColumn id="3" name="publiclyAvailable" dataDxfId="29">
       <calculatedColumnFormula>IF(MOD(ROW(),3)=0,"false","true")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{A4BCB875-2E6E-43F7-B0EE-9260BA7A5C65}" name="SQL" dataDxfId="27">
-      <calculatedColumnFormula>"insert into board (id, name, publicly_available) values ('"&amp;Tableau13[[#This Row],[id]]&amp;"', '"&amp;Tableau13[[#This Row],[name]]&amp;"', " &amp; Tableau13[[#This Row],[publiclyAvailable]] &amp; ");"</calculatedColumnFormula>
+    <tableColumn id="6" name="SQL" dataDxfId="1">
+      <calculatedColumnFormula>"insert into board (id, name, publicly_available) values ("&amp;Tableau13[[#This Row],[id]]&amp;", '"&amp;Tableau13[[#This Row],[name]]&amp;"', " &amp; Tableau13[[#This Row],[publiclyAvailable]] &amp; ");"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -595,38 +590,38 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{197C08B6-2888-4023-B8C4-C60AAFB68634}" name="Tableau14" displayName="Tableau14" ref="A1:J45" totalsRowShown="0" headerRowDxfId="26">
-  <autoFilter ref="A1:J45" xr:uid="{9AB14CFA-62D4-4A0B-93A0-BBF925029E3D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau14" displayName="Tableau14" ref="A1:J45" totalsRowShown="0" headerRowDxfId="28">
+  <autoFilter ref="A1:J45"/>
   <tableColumns count="10">
-    <tableColumn id="7" xr3:uid="{9E07FAB6-2ED5-4A2D-9038-C27CDD295494}" name="num ligne" dataDxfId="25">
+    <tableColumn id="7" name="num ligne" dataDxfId="27">
       <calculatedColumnFormula>ROW()-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{2CA62255-3F30-42C4-9A88-D52818CB60EF}" name="id" dataDxfId="24">
+    <tableColumn id="1" name="id" dataDxfId="26">
       <calculatedColumnFormula>Tableau14[[#This Row],[num ligne]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{9C84FF56-8BE1-45CA-B202-7DCA3C860668}" name="board_id" dataDxfId="23">
+    <tableColumn id="2" name="board_id" dataDxfId="25">
       <calculatedColumnFormula>1+MOD(ROW()-2,MAX(board!A:A))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{7F7513A1-E178-4938-BE53-76494ED4D60D}" name="date" dataDxfId="0">
+    <tableColumn id="3" name="date" dataDxfId="24">
       <calculatedColumnFormula>params!$B$3-ROW()+MOD(ROW(),23)/24 +MOD(ROW()+44,60)/24/60</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{E56F4E02-3A00-401C-A908-1A4BB5E9527A}" name="author_id" dataDxfId="22">
+    <tableColumn id="4" name="author_id" dataDxfId="23">
       <calculatedColumnFormula>1+MOD(ROW()-2,MAX(member!A:A))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{27A149DE-4A94-4CE3-BCAC-BE3643DB2536}" name="publiclyAvailable" dataDxfId="21">
+    <tableColumn id="5" name="publiclyAvailable" dataDxfId="22">
       <calculatedColumnFormula>IF(MOD(ROW(),10)=0,"false","true")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{3F78A448-4DB4-4FAB-BE21-F7DAE2611C4F}" name="nbPosts" dataDxfId="20">
+    <tableColumn id="8" name="nbPosts" dataDxfId="21">
       <calculatedColumnFormula>Tableau14[[#This Row],[num ligne]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{CDCB6001-F478-43AF-A5F0-D500E4FDA637}" name="title" dataDxfId="19">
+    <tableColumn id="9" name="title" dataDxfId="20">
       <calculatedColumnFormula>"The title of &lt;" &amp; Tableau14[[#This Row],[id]] &amp; "&gt;"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{902D888A-A354-4025-B1A4-08F503BE6D07}" name="content" dataDxfId="18">
+    <tableColumn id="10" name="content" dataDxfId="19">
       <calculatedColumnFormula>"The content of the topic &lt;" &amp; Tableau14[[#This Row],[id]] &amp; "&gt;"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{C418F970-327C-4413-BD7B-4F5E7512DCF3}" name="SQL" dataDxfId="17">
-      <calculatedColumnFormula>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('" &amp; B2 &amp; "', '" &amp; C2 &amp; "', '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', '" &amp; Tableau14[[#This Row],[author_id]] &amp; "', " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</calculatedColumnFormula>
+    <tableColumn id="6" name="SQL" dataDxfId="0">
+      <calculatedColumnFormula>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (" &amp; B2 &amp; ", " &amp; C2 &amp; ", '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', " &amp; Tableau14[[#This Row],[author_id]] &amp; ", " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -634,34 +629,34 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9DC02726-0965-4E3A-A891-C0BE8C94265C}" name="Tableau146" displayName="Tableau146" ref="A1:I321" totalsRowShown="0" headerRowDxfId="16">
-  <autoFilter ref="A1:I321" xr:uid="{4D78B567-D9F5-43BE-8FA8-EEA0152EAC04}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tableau146" displayName="Tableau146" ref="A1:I321" totalsRowShown="0" headerRowDxfId="18">
+  <autoFilter ref="A1:I321"/>
   <tableColumns count="9">
-    <tableColumn id="7" xr3:uid="{4A260F07-96E5-4472-8B48-83497FA72480}" name="num ligne" dataDxfId="15">
+    <tableColumn id="7" name="num ligne" dataDxfId="17">
       <calculatedColumnFormula>ROW()-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{52186376-6B5F-4AE1-A9C7-F6B1E50C9C81}" name="id" dataDxfId="14">
+    <tableColumn id="1" name="id" dataDxfId="16">
       <calculatedColumnFormula>Tableau146[[#This Row],[num ligne]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{481C429A-03DC-4A63-A353-2069EBDCB127}" name="topic_id" dataDxfId="13">
+    <tableColumn id="2" name="topic_id" dataDxfId="15">
       <calculatedColumnFormula>1+MOD(ROW()-2,MAX(topic!A:A))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{2B5E6132-0314-403F-8175-7BFF2CC41717}" name="date" dataDxfId="1">
+    <tableColumn id="3" name="date" dataDxfId="14">
       <calculatedColumnFormula>params!$B$3-ROW()+MOD(ROW(),23)/24 +MOD(ROW()+44,60)/24/60</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{C08E182F-1D7A-4EEF-B99E-2482901DB56B}" name="author_id" dataDxfId="12">
+    <tableColumn id="4" name="author_id" dataDxfId="13">
       <calculatedColumnFormula>1+MOD(ROW()-2,MAX(member!A:A))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{A466DCD5-B0A9-4CF9-AE0B-9CFCCF17E044}" name="publiclyAvailable" dataDxfId="11">
+    <tableColumn id="5" name="publiclyAvailable" dataDxfId="12">
       <calculatedColumnFormula>IF(MOD(ROW(),10)=0,"false","true")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{FDA69B6D-F462-43BB-A323-0DEC845EEDE2}" name="title" dataDxfId="10">
+    <tableColumn id="9" name="title" dataDxfId="11">
       <calculatedColumnFormula>"The title of &lt;" &amp; Tableau146[[#This Row],[id]] &amp; "&gt;"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{5A3A09C2-233F-4C01-8728-5AF740388EAF}" name="content" dataDxfId="9">
+    <tableColumn id="10" name="content" dataDxfId="10">
       <calculatedColumnFormula>"The content of the post &lt;" &amp; Tableau146[[#This Row],[id]] &amp; "&gt;"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{29F9A9FE-D2CC-4592-80FC-7FA674B3D116}" name="SQL" dataDxfId="8">
+    <tableColumn id="6" name="SQL" dataDxfId="9">
       <calculatedColumnFormula>"insert into post (id, topic_id, date, author_id, publicly_available, title, content) values (" &amp; B2 &amp; ", " &amp; C2 &amp; ", '" &amp; TEXT(Tableau146[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', " &amp; Tableau146[[#This Row],[author_id]] &amp; ", " &amp; Tableau146[[#This Row],[publiclyAvailable]] &amp; ", '" &amp; Tableau146[[#This Row],[title]] &amp; "', '" &amp; Tableau146[[#This Row],[content]] &amp; "');"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -670,25 +665,25 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{3CE3EF75-418B-402F-901F-AF96ECB6E239}" name="Tableau6" displayName="Tableau6" ref="A1:F529" totalsRowShown="0">
-  <autoFilter ref="A1:F529" xr:uid="{2E062A18-2A1D-43B1-B0CC-07A556999806}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tableau6" displayName="Tableau6" ref="A1:F529" totalsRowShown="0">
+  <autoFilter ref="A1:F529"/>
   <tableColumns count="6">
-    <tableColumn id="3" xr3:uid="{A8AF197B-18FA-480F-8349-F47AFD3F2805}" name="numLigne" dataDxfId="7">
+    <tableColumn id="3" name="numLigne" dataDxfId="8">
       <calculatedColumnFormula>ROW()-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{02F56E9B-8D2B-40DD-B2EA-F0853346B599}" name="isMember ?" dataDxfId="6">
+    <tableColumn id="1" name="isMember ?" dataDxfId="7">
       <calculatedColumnFormula>IF(Tableau6[[#This Row],[numLigne]] &lt;= MAX(member!A:A), "member!G" &amp; (Tableau6[[#This Row],[numLigne]]+1), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{E18319EE-4CAB-43E4-B409-EBB53CC0198D}" name="isBoard" dataDxfId="5">
+    <tableColumn id="2" name="isBoard" dataDxfId="6">
       <calculatedColumnFormula>IF(  OR(        ROW()&lt;=MAX(member!A:A)+1, ROW() &gt; MAX(member!A:A) + MAX(board!A:A) + 1),    "",  "board!E" &amp; (Tableau6[[#This Row],[numLigne]]-MAX(member!A:A)+1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{C67DCA99-ED19-44A0-A0C6-91FDF7A5C1AD}" name="isTopic" dataDxfId="4">
+    <tableColumn id="4" name="isTopic" dataDxfId="5">
       <calculatedColumnFormula>IF(  OR(        ROW()&lt;=MAX(member!A:A)+MAX(board!A:A)+1, ROW() &gt; MAX(member!A:A) + MAX(board!A:A) + MAX(topic!A:A) + 1),    "",  "topic!J" &amp; (Tableau6[[#This Row],[numLigne]]-MAX(member!A:A)-MAX(board!A:A)+1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{91099A80-62BC-4063-BBE7-4FAC9116201F}" name="isPost" dataDxfId="3">
+    <tableColumn id="5" name="isPost" dataDxfId="4">
       <calculatedColumnFormula>IF(  OR(        ROW()&lt;=MAX(member!A:A)+MAX(board!A:A)+ MAX(topic!A:A) +1, ROW() &gt; MAX(member!A:A) + MAX(board!A:A) + MAX(topic!A:A)+ MAX(post!A:A)  + 1),    "",  "post!I" &amp; (Tableau6[[#This Row],[numLigne]]-MAX(member!A:A)-MAX(board!A:A)- MAX(topic!A:A) +1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{B33269AE-8676-4AD2-98E6-7E56963EE564}" name="/* data.sql */" dataDxfId="2">
+    <tableColumn id="6" name="/* data.sql */" dataDxfId="3">
       <calculatedColumnFormula>IF( OR(F1="commit;",F1=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -958,7 +953,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB70B995-C22A-444B-9B6F-08C9DB8123B9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -984,11 +979,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1050,8 +1045,8 @@
         <v>7</v>
       </c>
       <c r="G2" t="str">
-        <f>"insert into member (id, name, alias, email, type) values ('"&amp;B2&amp;"', '"&amp;C2&amp;"', "&amp;IF(D2="null","null","'" &amp; D2 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('1', 'Name 1', null, 'name.1@graphql-java.com', 'ADMIN'); </v>
+        <f>"insert into member (id, name, alias, email, type) values ("&amp;B2&amp;", '"&amp;C2&amp;"', "&amp;IF(D2="null","null","'" &amp; D2 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (1, 'Name 1', null, 'name.1@graphql-java.com', 'ADMIN'); </v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -1078,8 +1073,8 @@
         <v>8</v>
       </c>
       <c r="G3" t="str">
-        <f>"insert into member (id, name, alias, email, type) values ('"&amp;B3&amp;"', '"&amp;C3&amp;"', "&amp;IF(D3="null","null","'" &amp; D3 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('2', 'Name 2', 'Alias of Name 2', 'name.2@graphql-java.com', 'MODERATOR'); </v>
+        <f>"insert into member (id, name, alias, email, type) values ("&amp;B3&amp;", '"&amp;C3&amp;"', "&amp;IF(D3="null","null","'" &amp; D3 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (2, 'Name 2', 'Alias of Name 2', 'name.2@graphql-java.com', 'MODERATOR'); </v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -1106,8 +1101,8 @@
         <v>9</v>
       </c>
       <c r="G4" t="str">
-        <f>"insert into member (id, name, alias, email, type) values ('"&amp;B4&amp;"', '"&amp;C4&amp;"', "&amp;IF(D4="null","null","'" &amp; D4 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('3', 'Name 3', null, 'name.3@graphql-java.com', 'STANDARD'); </v>
+        <f>"insert into member (id, name, alias, email, type) values ("&amp;B4&amp;", '"&amp;C4&amp;"', "&amp;IF(D4="null","null","'" &amp; D4 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (3, 'Name 3', null, 'name.3@graphql-java.com', 'STANDARD'); </v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -1134,8 +1129,8 @@
         <v>7</v>
       </c>
       <c r="G5" t="str">
-        <f>"insert into member (id, name, alias, email, type) values ('"&amp;B5&amp;"', '"&amp;C5&amp;"', "&amp;IF(D5="null","null","'" &amp; D5 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('4', 'Name 4', 'Alias of Name 4', 'name.4@graphql-java.com', 'ADMIN'); </v>
+        <f>"insert into member (id, name, alias, email, type) values ("&amp;B5&amp;", '"&amp;C5&amp;"', "&amp;IF(D5="null","null","'" &amp; D5 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (4, 'Name 4', 'Alias of Name 4', 'name.4@graphql-java.com', 'ADMIN'); </v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1162,8 +1157,8 @@
         <v>8</v>
       </c>
       <c r="G6" t="str">
-        <f>"insert into member (id, name, alias, email, type) values ('"&amp;B6&amp;"', '"&amp;C6&amp;"', "&amp;IF(D6="null","null","'" &amp; D6 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('5', 'Name 5', null, 'name.5@graphql-java.com', 'MODERATOR'); </v>
+        <f>"insert into member (id, name, alias, email, type) values ("&amp;B6&amp;", '"&amp;C6&amp;"', "&amp;IF(D6="null","null","'" &amp; D6 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (5, 'Name 5', null, 'name.5@graphql-java.com', 'MODERATOR'); </v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -1190,8 +1185,8 @@
         <v>9</v>
       </c>
       <c r="G7" t="str">
-        <f>"insert into member (id, name, alias, email, type) values ('"&amp;B7&amp;"', '"&amp;C7&amp;"', "&amp;IF(D7="null","null","'" &amp; D7 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('6', 'Name 6', 'Alias of Name 6', 'name.6@graphql-java.com', 'STANDARD'); </v>
+        <f>"insert into member (id, name, alias, email, type) values ("&amp;B7&amp;", '"&amp;C7&amp;"', "&amp;IF(D7="null","null","'" &amp; D7 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (6, 'Name 6', 'Alias of Name 6', 'name.6@graphql-java.com', 'STANDARD'); </v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -1218,8 +1213,8 @@
         <v>7</v>
       </c>
       <c r="G8" t="str">
-        <f>"insert into member (id, name, alias, email, type) values ('"&amp;B8&amp;"', '"&amp;C8&amp;"', "&amp;IF(D8="null","null","'" &amp; D8 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('7', 'Name 7', null, 'name.7@graphql-java.com', 'ADMIN'); </v>
+        <f>"insert into member (id, name, alias, email, type) values ("&amp;B8&amp;", '"&amp;C8&amp;"', "&amp;IF(D8="null","null","'" &amp; D8 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (7, 'Name 7', null, 'name.7@graphql-java.com', 'ADMIN'); </v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -1246,8 +1241,8 @@
         <v>8</v>
       </c>
       <c r="G9" t="str">
-        <f>"insert into member (id, name, alias, email, type) values ('"&amp;B9&amp;"', '"&amp;C9&amp;"', "&amp;IF(D9="null","null","'" &amp; D9 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('8', 'Name 8', 'Alias of Name 8', 'name.8@graphql-java.com', 'MODERATOR'); </v>
+        <f>"insert into member (id, name, alias, email, type) values ("&amp;B9&amp;", '"&amp;C9&amp;"', "&amp;IF(D9="null","null","'" &amp; D9 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (8, 'Name 8', 'Alias of Name 8', 'name.8@graphql-java.com', 'MODERATOR'); </v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -1274,8 +1269,8 @@
         <v>9</v>
       </c>
       <c r="G10" t="str">
-        <f>"insert into member (id, name, alias, email, type) values ('"&amp;B10&amp;"', '"&amp;C10&amp;"', "&amp;IF(D10="null","null","'" &amp; D10 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('9', 'Name 9', null, 'name.9@graphql-java.com', 'STANDARD'); </v>
+        <f>"insert into member (id, name, alias, email, type) values ("&amp;B10&amp;", '"&amp;C10&amp;"', "&amp;IF(D10="null","null","'" &amp; D10 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (9, 'Name 9', null, 'name.9@graphql-java.com', 'STANDARD'); </v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -1302,8 +1297,8 @@
         <v>7</v>
       </c>
       <c r="G11" t="str">
-        <f>"insert into member (id, name, alias, email, type) values ('"&amp;B11&amp;"', '"&amp;C11&amp;"', "&amp;IF(D11="null","null","'" &amp; D11 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('10', 'Name 10', 'Alias of Name 10', 'name.10@graphql-java.com', 'ADMIN'); </v>
+        <f>"insert into member (id, name, alias, email, type) values ("&amp;B11&amp;", '"&amp;C11&amp;"', "&amp;IF(D11="null","null","'" &amp; D11 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (10, 'Name 10', 'Alias of Name 10', 'name.10@graphql-java.com', 'ADMIN'); </v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -1330,8 +1325,8 @@
         <v>8</v>
       </c>
       <c r="G12" t="str">
-        <f>"insert into member (id, name, alias, email, type) values ('"&amp;B12&amp;"', '"&amp;C12&amp;"', "&amp;IF(D12="null","null","'" &amp; D12 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('11', 'Name 11', null, 'name.11@graphql-java.com', 'MODERATOR'); </v>
+        <f>"insert into member (id, name, alias, email, type) values ("&amp;B12&amp;", '"&amp;C12&amp;"', "&amp;IF(D12="null","null","'" &amp; D12 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (11, 'Name 11', null, 'name.11@graphql-java.com', 'MODERATOR'); </v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -1358,8 +1353,8 @@
         <v>9</v>
       </c>
       <c r="G13" t="str">
-        <f>"insert into member (id, name, alias, email, type) values ('"&amp;B13&amp;"', '"&amp;C13&amp;"', "&amp;IF(D13="null","null","'" &amp; D13 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('12', 'Name 12', 'Alias of Name 12', 'name.12@graphql-java.com', 'STANDARD'); </v>
+        <f>"insert into member (id, name, alias, email, type) values ("&amp;B13&amp;", '"&amp;C13&amp;"', "&amp;IF(D13="null","null","'" &amp; D13 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (12, 'Name 12', 'Alias of Name 12', 'name.12@graphql-java.com', 'STANDARD'); </v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -1386,8 +1381,8 @@
         <v>7</v>
       </c>
       <c r="G14" t="str">
-        <f>"insert into member (id, name, alias, email, type) values ('"&amp;B14&amp;"', '"&amp;C14&amp;"', "&amp;IF(D14="null","null","'" &amp; D14 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('13', 'Name 13', null, 'name.13@graphql-java.com', 'ADMIN'); </v>
+        <f>"insert into member (id, name, alias, email, type) values ("&amp;B14&amp;", '"&amp;C14&amp;"', "&amp;IF(D14="null","null","'" &amp; D14 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (13, 'Name 13', null, 'name.13@graphql-java.com', 'ADMIN'); </v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -1414,8 +1409,8 @@
         <v>8</v>
       </c>
       <c r="G15" t="str">
-        <f>"insert into member (id, name, alias, email, type) values ('"&amp;B15&amp;"', '"&amp;C15&amp;"', "&amp;IF(D15="null","null","'" &amp; D15 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('14', 'Name 14', 'Alias of Name 14', 'name.14@graphql-java.com', 'MODERATOR'); </v>
+        <f>"insert into member (id, name, alias, email, type) values ("&amp;B15&amp;", '"&amp;C15&amp;"', "&amp;IF(D15="null","null","'" &amp; D15 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (14, 'Name 14', 'Alias of Name 14', 'name.14@graphql-java.com', 'MODERATOR'); </v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -1442,8 +1437,8 @@
         <v>9</v>
       </c>
       <c r="G16" t="str">
-        <f>"insert into member (id, name, alias, email, type) values ('"&amp;B16&amp;"', '"&amp;C16&amp;"', "&amp;IF(D16="null","null","'" &amp; D16 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('15', 'Name 15', null, 'name.15@graphql-java.com', 'STANDARD'); </v>
+        <f>"insert into member (id, name, alias, email, type) values ("&amp;B16&amp;", '"&amp;C16&amp;"', "&amp;IF(D16="null","null","'" &amp; D16 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (15, 'Name 15', null, 'name.15@graphql-java.com', 'STANDARD'); </v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -1470,8 +1465,8 @@
         <v>7</v>
       </c>
       <c r="G17" t="str">
-        <f>"insert into member (id, name, alias, email, type) values ('"&amp;B17&amp;"', '"&amp;C17&amp;"', "&amp;IF(D17="null","null","'" &amp; D17 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('16', 'Name 16', 'Alias of Name 16', 'name.16@graphql-java.com', 'ADMIN'); </v>
+        <f>"insert into member (id, name, alias, email, type) values ("&amp;B17&amp;", '"&amp;C17&amp;"', "&amp;IF(D17="null","null","'" &amp; D17 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (16, 'Name 16', 'Alias of Name 16', 'name.16@graphql-java.com', 'ADMIN'); </v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -1498,8 +1493,8 @@
         <v>8</v>
       </c>
       <c r="G18" t="str">
-        <f>"insert into member (id, name, alias, email, type) values ('"&amp;B18&amp;"', '"&amp;C18&amp;"', "&amp;IF(D18="null","null","'" &amp; D18 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('17', 'Name 17', null, 'name.17@graphql-java.com', 'MODERATOR'); </v>
+        <f>"insert into member (id, name, alias, email, type) values ("&amp;B18&amp;", '"&amp;C18&amp;"', "&amp;IF(D18="null","null","'" &amp; D18 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (17, 'Name 17', null, 'name.17@graphql-java.com', 'MODERATOR'); </v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -1526,8 +1521,8 @@
         <v>9</v>
       </c>
       <c r="G19" t="str">
-        <f>"insert into member (id, name, alias, email, type) values ('"&amp;B19&amp;"', '"&amp;C19&amp;"', "&amp;IF(D19="null","null","'" &amp; D19 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('18', 'Name 18', 'Alias of Name 18', 'name.18@graphql-java.com', 'STANDARD'); </v>
+        <f>"insert into member (id, name, alias, email, type) values ("&amp;B19&amp;", '"&amp;C19&amp;"', "&amp;IF(D19="null","null","'" &amp; D19 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (18, 'Name 18', 'Alias of Name 18', 'name.18@graphql-java.com', 'STANDARD'); </v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -1554,8 +1549,8 @@
         <v>7</v>
       </c>
       <c r="G20" t="str">
-        <f>"insert into member (id, name, alias, email, type) values ('"&amp;B20&amp;"', '"&amp;C20&amp;"', "&amp;IF(D20="null","null","'" &amp; D20 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('19', 'Name 19', null, 'name.19@graphql-java.com', 'ADMIN'); </v>
+        <f>"insert into member (id, name, alias, email, type) values ("&amp;B20&amp;", '"&amp;C20&amp;"', "&amp;IF(D20="null","null","'" &amp; D20 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (19, 'Name 19', null, 'name.19@graphql-java.com', 'ADMIN'); </v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -1582,8 +1577,8 @@
         <v>8</v>
       </c>
       <c r="G21" t="str">
-        <f>"insert into member (id, name, alias, email, type) values ('"&amp;B21&amp;"', '"&amp;C21&amp;"', "&amp;IF(D21="null","null","'" &amp; D21 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('20', 'Name 20', 'Alias of Name 20', 'name.20@graphql-java.com', 'MODERATOR'); </v>
+        <f>"insert into member (id, name, alias, email, type) values ("&amp;B21&amp;", '"&amp;C21&amp;"', "&amp;IF(D21="null","null","'" &amp; D21 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (20, 'Name 20', 'Alias of Name 20', 'name.20@graphql-java.com', 'MODERATOR'); </v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -1610,8 +1605,8 @@
         <v>9</v>
       </c>
       <c r="G22" t="str">
-        <f>"insert into member (id, name, alias, email, type) values ('"&amp;B22&amp;"', '"&amp;C22&amp;"', "&amp;IF(D22="null","null","'" &amp; D22 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('21', 'Name 21', null, 'name.21@graphql-java.com', 'STANDARD'); </v>
+        <f>"insert into member (id, name, alias, email, type) values ("&amp;B22&amp;", '"&amp;C22&amp;"', "&amp;IF(D22="null","null","'" &amp; D22 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (21, 'Name 21', null, 'name.21@graphql-java.com', 'STANDARD'); </v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -1638,8 +1633,8 @@
         <v>7</v>
       </c>
       <c r="G23" t="str">
-        <f>"insert into member (id, name, alias, email, type) values ('"&amp;B23&amp;"', '"&amp;C23&amp;"', "&amp;IF(D23="null","null","'" &amp; D23 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('22', 'Name 22', 'Alias of Name 22', 'name.22@graphql-java.com', 'ADMIN'); </v>
+        <f>"insert into member (id, name, alias, email, type) values ("&amp;B23&amp;", '"&amp;C23&amp;"', "&amp;IF(D23="null","null","'" &amp; D23 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (22, 'Name 22', 'Alias of Name 22', 'name.22@graphql-java.com', 'ADMIN'); </v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
@@ -1666,8 +1661,8 @@
         <v>8</v>
       </c>
       <c r="G24" t="str">
-        <f>"insert into member (id, name, alias, email, type) values ('"&amp;B24&amp;"', '"&amp;C24&amp;"', "&amp;IF(D24="null","null","'" &amp; D24 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('23', 'Name 23', null, 'name.23@graphql-java.com', 'MODERATOR'); </v>
+        <f>"insert into member (id, name, alias, email, type) values ("&amp;B24&amp;", '"&amp;C24&amp;"', "&amp;IF(D24="null","null","'" &amp; D24 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (23, 'Name 23', null, 'name.23@graphql-java.com', 'MODERATOR'); </v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -1694,8 +1689,8 @@
         <v>9</v>
       </c>
       <c r="G25" t="str">
-        <f>"insert into member (id, name, alias, email, type) values ('"&amp;B25&amp;"', '"&amp;C25&amp;"', "&amp;IF(D25="null","null","'" &amp; D25 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('24', 'Name 24', 'Alias of Name 24', 'name.24@graphql-java.com', 'STANDARD'); </v>
+        <f>"insert into member (id, name, alias, email, type) values ("&amp;B25&amp;", '"&amp;C25&amp;"', "&amp;IF(D25="null","null","'" &amp; D25 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (24, 'Name 24', 'Alias of Name 24', 'name.24@graphql-java.com', 'STANDARD'); </v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -1722,8 +1717,8 @@
         <v>7</v>
       </c>
       <c r="G26" t="str">
-        <f>"insert into member (id, name, alias, email, type) values ('"&amp;B26&amp;"', '"&amp;C26&amp;"', "&amp;IF(D26="null","null","'" &amp; D26 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('25', 'Name 25', null, 'name.25@graphql-java.com', 'ADMIN'); </v>
+        <f>"insert into member (id, name, alias, email, type) values ("&amp;B26&amp;", '"&amp;C26&amp;"', "&amp;IF(D26="null","null","'" &amp; D26 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (25, 'Name 25', null, 'name.25@graphql-java.com', 'ADMIN'); </v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -1750,8 +1745,8 @@
         <v>8</v>
       </c>
       <c r="G27" t="str">
-        <f>"insert into member (id, name, alias, email, type) values ('"&amp;B27&amp;"', '"&amp;C27&amp;"', "&amp;IF(D27="null","null","'" &amp; D27 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('26', 'Name 26', 'Alias of Name 26', 'name.26@graphql-java.com', 'MODERATOR'); </v>
+        <f>"insert into member (id, name, alias, email, type) values ("&amp;B27&amp;", '"&amp;C27&amp;"', "&amp;IF(D27="null","null","'" &amp; D27 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (26, 'Name 26', 'Alias of Name 26', 'name.26@graphql-java.com', 'MODERATOR'); </v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -1778,8 +1773,8 @@
         <v>9</v>
       </c>
       <c r="G28" t="str">
-        <f>"insert into member (id, name, alias, email, type) values ('"&amp;B28&amp;"', '"&amp;C28&amp;"', "&amp;IF(D28="null","null","'" &amp; D28 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('27', 'Name 27', null, 'name.27@graphql-java.com', 'STANDARD'); </v>
+        <f>"insert into member (id, name, alias, email, type) values ("&amp;B28&amp;", '"&amp;C28&amp;"', "&amp;IF(D28="null","null","'" &amp; D28 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (27, 'Name 27', null, 'name.27@graphql-java.com', 'STANDARD'); </v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
@@ -1806,8 +1801,8 @@
         <v>7</v>
       </c>
       <c r="G29" t="str">
-        <f>"insert into member (id, name, alias, email, type) values ('"&amp;B29&amp;"', '"&amp;C29&amp;"', "&amp;IF(D29="null","null","'" &amp; D29 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('28', 'Name 28', 'Alias of Name 28', 'name.28@graphql-java.com', 'ADMIN'); </v>
+        <f>"insert into member (id, name, alias, email, type) values ("&amp;B29&amp;", '"&amp;C29&amp;"', "&amp;IF(D29="null","null","'" &amp; D29 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (28, 'Name 28', 'Alias of Name 28', 'name.28@graphql-java.com', 'ADMIN'); </v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
@@ -1834,8 +1829,8 @@
         <v>8</v>
       </c>
       <c r="G30" t="str">
-        <f>"insert into member (id, name, alias, email, type) values ('"&amp;B30&amp;"', '"&amp;C30&amp;"', "&amp;IF(D30="null","null","'" &amp; D30 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('29', 'Name 29', null, 'name.29@graphql-java.com', 'MODERATOR'); </v>
+        <f>"insert into member (id, name, alias, email, type) values ("&amp;B30&amp;", '"&amp;C30&amp;"', "&amp;IF(D30="null","null","'" &amp; D30 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (29, 'Name 29', null, 'name.29@graphql-java.com', 'MODERATOR'); </v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
@@ -1862,8 +1857,8 @@
         <v>9</v>
       </c>
       <c r="G31" t="str">
-        <f>"insert into member (id, name, alias, email, type) values ('"&amp;B31&amp;"', '"&amp;C31&amp;"', "&amp;IF(D31="null","null","'" &amp; D31 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('30', 'Name 30', 'Alias of Name 30', 'name.30@graphql-java.com', 'STANDARD'); </v>
+        <f>"insert into member (id, name, alias, email, type) values ("&amp;B31&amp;", '"&amp;C31&amp;"', "&amp;IF(D31="null","null","'" &amp; D31 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (30, 'Name 30', 'Alias of Name 30', 'name.30@graphql-java.com', 'STANDARD'); </v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
@@ -1890,8 +1885,8 @@
         <v>7</v>
       </c>
       <c r="G32" t="str">
-        <f>"insert into member (id, name, alias, email, type) values ('"&amp;B32&amp;"', '"&amp;C32&amp;"', "&amp;IF(D32="null","null","'" &amp; D32 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('31', 'Name 31', null, 'name.31@graphql-java.com', 'ADMIN'); </v>
+        <f>"insert into member (id, name, alias, email, type) values ("&amp;B32&amp;", '"&amp;C32&amp;"', "&amp;IF(D32="null","null","'" &amp; D32 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (31, 'Name 31', null, 'name.31@graphql-java.com', 'ADMIN'); </v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -1918,8 +1913,8 @@
         <v>8</v>
       </c>
       <c r="G33" t="str">
-        <f>"insert into member (id, name, alias, email, type) values ('"&amp;B33&amp;"', '"&amp;C33&amp;"', "&amp;IF(D33="null","null","'" &amp; D33 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('32', 'Name 32', 'Alias of Name 32', 'name.32@graphql-java.com', 'MODERATOR'); </v>
+        <f>"insert into member (id, name, alias, email, type) values ("&amp;B33&amp;", '"&amp;C33&amp;"', "&amp;IF(D33="null","null","'" &amp; D33 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (32, 'Name 32', 'Alias of Name 32', 'name.32@graphql-java.com', 'MODERATOR'); </v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -1946,8 +1941,8 @@
         <v>9</v>
       </c>
       <c r="G34" t="str">
-        <f>"insert into member (id, name, alias, email, type) values ('"&amp;B34&amp;"', '"&amp;C34&amp;"', "&amp;IF(D34="null","null","'" &amp; D34 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('33', 'Name 33', null, 'name.33@graphql-java.com', 'STANDARD'); </v>
+        <f>"insert into member (id, name, alias, email, type) values ("&amp;B34&amp;", '"&amp;C34&amp;"', "&amp;IF(D34="null","null","'" &amp; D34 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (33, 'Name 33', null, 'name.33@graphql-java.com', 'STANDARD'); </v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -1974,8 +1969,8 @@
         <v>7</v>
       </c>
       <c r="G35" t="str">
-        <f>"insert into member (id, name, alias, email, type) values ('"&amp;B35&amp;"', '"&amp;C35&amp;"', "&amp;IF(D35="null","null","'" &amp; D35 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('34', 'Name 34', 'Alias of Name 34', 'name.34@graphql-java.com', 'ADMIN'); </v>
+        <f>"insert into member (id, name, alias, email, type) values ("&amp;B35&amp;", '"&amp;C35&amp;"', "&amp;IF(D35="null","null","'" &amp; D35 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (34, 'Name 34', 'Alias of Name 34', 'name.34@graphql-java.com', 'ADMIN'); </v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
@@ -2002,8 +1997,8 @@
         <v>8</v>
       </c>
       <c r="G36" t="str">
-        <f>"insert into member (id, name, alias, email, type) values ('"&amp;B36&amp;"', '"&amp;C36&amp;"', "&amp;IF(D36="null","null","'" &amp; D36 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('35', 'Name 35', null, 'name.35@graphql-java.com', 'MODERATOR'); </v>
+        <f>"insert into member (id, name, alias, email, type) values ("&amp;B36&amp;", '"&amp;C36&amp;"', "&amp;IF(D36="null","null","'" &amp; D36 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (35, 'Name 35', null, 'name.35@graphql-java.com', 'MODERATOR'); </v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -2030,8 +2025,8 @@
         <v>9</v>
       </c>
       <c r="G37" t="str">
-        <f>"insert into member (id, name, alias, email, type) values ('"&amp;B37&amp;"', '"&amp;C37&amp;"', "&amp;IF(D37="null","null","'" &amp; D37 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('36', 'Name 36', 'Alias of Name 36', 'name.36@graphql-java.com', 'STANDARD'); </v>
+        <f>"insert into member (id, name, alias, email, type) values ("&amp;B37&amp;", '"&amp;C37&amp;"', "&amp;IF(D37="null","null","'" &amp; D37 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (36, 'Name 36', 'Alias of Name 36', 'name.36@graphql-java.com', 'STANDARD'); </v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -2058,8 +2053,8 @@
         <v>7</v>
       </c>
       <c r="G38" t="str">
-        <f>"insert into member (id, name, alias, email, type) values ('"&amp;B38&amp;"', '"&amp;C38&amp;"', "&amp;IF(D38="null","null","'" &amp; D38 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('37', 'Name 37', null, 'name.37@graphql-java.com', 'ADMIN'); </v>
+        <f>"insert into member (id, name, alias, email, type) values ("&amp;B38&amp;", '"&amp;C38&amp;"', "&amp;IF(D38="null","null","'" &amp; D38 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (37, 'Name 37', null, 'name.37@graphql-java.com', 'ADMIN'); </v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
@@ -2086,8 +2081,8 @@
         <v>8</v>
       </c>
       <c r="G39" t="str">
-        <f>"insert into member (id, name, alias, email, type) values ('"&amp;B39&amp;"', '"&amp;C39&amp;"', "&amp;IF(D39="null","null","'" &amp; D39 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('38', 'Name 38', 'Alias of Name 38', 'name.38@graphql-java.com', 'MODERATOR'); </v>
+        <f>"insert into member (id, name, alias, email, type) values ("&amp;B39&amp;", '"&amp;C39&amp;"', "&amp;IF(D39="null","null","'" &amp; D39 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (38, 'Name 38', 'Alias of Name 38', 'name.38@graphql-java.com', 'MODERATOR'); </v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
@@ -2114,8 +2109,8 @@
         <v>9</v>
       </c>
       <c r="G40" t="str">
-        <f>"insert into member (id, name, alias, email, type) values ('"&amp;B40&amp;"', '"&amp;C40&amp;"', "&amp;IF(D40="null","null","'" &amp; D40 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('39', 'Name 39', null, 'name.39@graphql-java.com', 'STANDARD'); </v>
+        <f>"insert into member (id, name, alias, email, type) values ("&amp;B40&amp;", '"&amp;C40&amp;"', "&amp;IF(D40="null","null","'" &amp; D40 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (39, 'Name 39', null, 'name.39@graphql-java.com', 'STANDARD'); </v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
@@ -2142,8 +2137,8 @@
         <v>7</v>
       </c>
       <c r="G41" t="str">
-        <f>"insert into member (id, name, alias, email, type) values ('"&amp;B41&amp;"', '"&amp;C41&amp;"', "&amp;IF(D41="null","null","'" &amp; D41 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('40', 'Name 40', 'Alias of Name 40', 'name.40@graphql-java.com', 'ADMIN'); </v>
+        <f>"insert into member (id, name, alias, email, type) values ("&amp;B41&amp;", '"&amp;C41&amp;"', "&amp;IF(D41="null","null","'" &amp; D41 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (40, 'Name 40', 'Alias of Name 40', 'name.40@graphql-java.com', 'ADMIN'); </v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
@@ -2170,8 +2165,8 @@
         <v>8</v>
       </c>
       <c r="G42" t="str">
-        <f>"insert into member (id, name, alias, email, type) values ('"&amp;B42&amp;"', '"&amp;C42&amp;"', "&amp;IF(D42="null","null","'" &amp; D42 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('41', 'Name 41', null, 'name.41@graphql-java.com', 'MODERATOR'); </v>
+        <f>"insert into member (id, name, alias, email, type) values ("&amp;B42&amp;", '"&amp;C42&amp;"', "&amp;IF(D42="null","null","'" &amp; D42 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (41, 'Name 41', null, 'name.41@graphql-java.com', 'MODERATOR'); </v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
@@ -2198,8 +2193,8 @@
         <v>9</v>
       </c>
       <c r="G43" t="str">
-        <f>"insert into member (id, name, alias, email, type) values ('"&amp;B43&amp;"', '"&amp;C43&amp;"', "&amp;IF(D43="null","null","'" &amp; D43 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('42', 'Name 42', 'Alias of Name 42', 'name.42@graphql-java.com', 'STANDARD'); </v>
+        <f>"insert into member (id, name, alias, email, type) values ("&amp;B43&amp;", '"&amp;C43&amp;"', "&amp;IF(D43="null","null","'" &amp; D43 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (42, 'Name 42', 'Alias of Name 42', 'name.42@graphql-java.com', 'STANDARD'); </v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
@@ -2226,8 +2221,8 @@
         <v>7</v>
       </c>
       <c r="G44" t="str">
-        <f>"insert into member (id, name, alias, email, type) values ('"&amp;B44&amp;"', '"&amp;C44&amp;"', "&amp;IF(D44="null","null","'" &amp; D44 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('43', 'Name 43', null, 'name.43@graphql-java.com', 'ADMIN'); </v>
+        <f>"insert into member (id, name, alias, email, type) values ("&amp;B44&amp;", '"&amp;C44&amp;"', "&amp;IF(D44="null","null","'" &amp; D44 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (43, 'Name 43', null, 'name.43@graphql-java.com', 'ADMIN'); </v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
@@ -2254,8 +2249,8 @@
         <v>8</v>
       </c>
       <c r="G45" t="str">
-        <f>"insert into member (id, name, alias, email, type) values ('"&amp;B45&amp;"', '"&amp;C45&amp;"', "&amp;IF(D45="null","null","'" &amp; D45 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('44', 'Name 44', 'Alias of Name 44', 'name.44@graphql-java.com', 'MODERATOR'); </v>
+        <f>"insert into member (id, name, alias, email, type) values ("&amp;B45&amp;", '"&amp;C45&amp;"', "&amp;IF(D45="null","null","'" &amp; D45 &amp; "'") &amp; ", '" &amp; Tableau1[[#This Row],[email]] &amp; "', '" &amp; Tableau1[[#This Row],[type]] &amp; "'); "</f>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (44, 'Name 44', 'Alias of Name 44', 'name.44@graphql-java.com', 'MODERATOR'); </v>
       </c>
     </row>
   </sheetData>
@@ -2268,11 +2263,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E043A28-5205-4979-8ACA-86EF67A794E6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2319,8 +2314,8 @@
         <v>true</v>
       </c>
       <c r="E2" t="str">
-        <f>"insert into board (id, name, publicly_available) values ('"&amp;Tableau13[[#This Row],[id]]&amp;"', '"&amp;Tableau13[[#This Row],[name]]&amp;"', " &amp; Tableau13[[#This Row],[publiclyAvailable]] &amp; ");"</f>
-        <v>insert into board (id, name, publicly_available) values ('1', 'Board name 1', true);</v>
+        <f>"insert into board (id, name, publicly_available) values ("&amp;Tableau13[[#This Row],[id]]&amp;", '"&amp;Tableau13[[#This Row],[name]]&amp;"', " &amp; Tableau13[[#This Row],[publiclyAvailable]] &amp; ");"</f>
+        <v>insert into board (id, name, publicly_available) values (1, 'Board name 1', true);</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -2340,8 +2335,8 @@
         <v>false</v>
       </c>
       <c r="E3" t="str">
-        <f>"insert into board (id, name, publicly_available) values ('"&amp;Tableau13[[#This Row],[id]]&amp;"', '"&amp;Tableau13[[#This Row],[name]]&amp;"', " &amp; Tableau13[[#This Row],[publiclyAvailable]] &amp; ");"</f>
-        <v>insert into board (id, name, publicly_available) values ('2', 'Board name 2', false);</v>
+        <f>"insert into board (id, name, publicly_available) values ("&amp;Tableau13[[#This Row],[id]]&amp;", '"&amp;Tableau13[[#This Row],[name]]&amp;"', " &amp; Tableau13[[#This Row],[publiclyAvailable]] &amp; ");"</f>
+        <v>insert into board (id, name, publicly_available) values (2, 'Board name 2', false);</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -2361,8 +2356,8 @@
         <v>true</v>
       </c>
       <c r="E4" t="str">
-        <f>"insert into board (id, name, publicly_available) values ('"&amp;Tableau13[[#This Row],[id]]&amp;"', '"&amp;Tableau13[[#This Row],[name]]&amp;"', " &amp; Tableau13[[#This Row],[publiclyAvailable]] &amp; ");"</f>
-        <v>insert into board (id, name, publicly_available) values ('3', 'Board name 3', true);</v>
+        <f>"insert into board (id, name, publicly_available) values ("&amp;Tableau13[[#This Row],[id]]&amp;", '"&amp;Tableau13[[#This Row],[name]]&amp;"', " &amp; Tableau13[[#This Row],[publiclyAvailable]] &amp; ");"</f>
+        <v>insert into board (id, name, publicly_available) values (3, 'Board name 3', true);</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -2382,8 +2377,8 @@
         <v>true</v>
       </c>
       <c r="E5" t="str">
-        <f>"insert into board (id, name, publicly_available) values ('"&amp;Tableau13[[#This Row],[id]]&amp;"', '"&amp;Tableau13[[#This Row],[name]]&amp;"', " &amp; Tableau13[[#This Row],[publiclyAvailable]] &amp; ");"</f>
-        <v>insert into board (id, name, publicly_available) values ('4', 'Board name 4', true);</v>
+        <f>"insert into board (id, name, publicly_available) values ("&amp;Tableau13[[#This Row],[id]]&amp;", '"&amp;Tableau13[[#This Row],[name]]&amp;"', " &amp; Tableau13[[#This Row],[publiclyAvailable]] &amp; ");"</f>
+        <v>insert into board (id, name, publicly_available) values (4, 'Board name 4', true);</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -2403,8 +2398,8 @@
         <v>false</v>
       </c>
       <c r="E6" t="str">
-        <f>"insert into board (id, name, publicly_available) values ('"&amp;Tableau13[[#This Row],[id]]&amp;"', '"&amp;Tableau13[[#This Row],[name]]&amp;"', " &amp; Tableau13[[#This Row],[publiclyAvailable]] &amp; ");"</f>
-        <v>insert into board (id, name, publicly_available) values ('5', 'Board name 5', false);</v>
+        <f>"insert into board (id, name, publicly_available) values ("&amp;Tableau13[[#This Row],[id]]&amp;", '"&amp;Tableau13[[#This Row],[name]]&amp;"', " &amp; Tableau13[[#This Row],[publiclyAvailable]] &amp; ");"</f>
+        <v>insert into board (id, name, publicly_available) values (5, 'Board name 5', false);</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -2424,8 +2419,8 @@
         <v>true</v>
       </c>
       <c r="E7" t="str">
-        <f>"insert into board (id, name, publicly_available) values ('"&amp;Tableau13[[#This Row],[id]]&amp;"', '"&amp;Tableau13[[#This Row],[name]]&amp;"', " &amp; Tableau13[[#This Row],[publiclyAvailable]] &amp; ");"</f>
-        <v>insert into board (id, name, publicly_available) values ('6', 'Board name 6', true);</v>
+        <f>"insert into board (id, name, publicly_available) values ("&amp;Tableau13[[#This Row],[id]]&amp;", '"&amp;Tableau13[[#This Row],[name]]&amp;"', " &amp; Tableau13[[#This Row],[publiclyAvailable]] &amp; ");"</f>
+        <v>insert into board (id, name, publicly_available) values (6, 'Board name 6', true);</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -2445,8 +2440,8 @@
         <v>true</v>
       </c>
       <c r="E8" t="str">
-        <f>"insert into board (id, name, publicly_available) values ('"&amp;Tableau13[[#This Row],[id]]&amp;"', '"&amp;Tableau13[[#This Row],[name]]&amp;"', " &amp; Tableau13[[#This Row],[publiclyAvailable]] &amp; ");"</f>
-        <v>insert into board (id, name, publicly_available) values ('7', 'Board name 7', true);</v>
+        <f>"insert into board (id, name, publicly_available) values ("&amp;Tableau13[[#This Row],[id]]&amp;", '"&amp;Tableau13[[#This Row],[name]]&amp;"', " &amp; Tableau13[[#This Row],[publiclyAvailable]] &amp; ");"</f>
+        <v>insert into board (id, name, publicly_available) values (7, 'Board name 7', true);</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -2466,8 +2461,8 @@
         <v>false</v>
       </c>
       <c r="E9" t="str">
-        <f>"insert into board (id, name, publicly_available) values ('"&amp;Tableau13[[#This Row],[id]]&amp;"', '"&amp;Tableau13[[#This Row],[name]]&amp;"', " &amp; Tableau13[[#This Row],[publiclyAvailable]] &amp; ");"</f>
-        <v>insert into board (id, name, publicly_available) values ('8', 'Board name 8', false);</v>
+        <f>"insert into board (id, name, publicly_available) values ("&amp;Tableau13[[#This Row],[id]]&amp;", '"&amp;Tableau13[[#This Row],[name]]&amp;"', " &amp; Tableau13[[#This Row],[publiclyAvailable]] &amp; ");"</f>
+        <v>insert into board (id, name, publicly_available) values (8, 'Board name 8', false);</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -2487,8 +2482,8 @@
         <v>true</v>
       </c>
       <c r="E10" t="str">
-        <f>"insert into board (id, name, publicly_available) values ('"&amp;Tableau13[[#This Row],[id]]&amp;"', '"&amp;Tableau13[[#This Row],[name]]&amp;"', " &amp; Tableau13[[#This Row],[publiclyAvailable]] &amp; ");"</f>
-        <v>insert into board (id, name, publicly_available) values ('9', 'Board name 9', true);</v>
+        <f>"insert into board (id, name, publicly_available) values ("&amp;Tableau13[[#This Row],[id]]&amp;", '"&amp;Tableau13[[#This Row],[name]]&amp;"', " &amp; Tableau13[[#This Row],[publiclyAvailable]] &amp; ");"</f>
+        <v>insert into board (id, name, publicly_available) values (9, 'Board name 9', true);</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -2508,8 +2503,8 @@
         <v>true</v>
       </c>
       <c r="E11" s="5" t="str">
-        <f>"insert into board (id, name, publicly_available) values ('"&amp;Tableau13[[#This Row],[id]]&amp;"', '"&amp;Tableau13[[#This Row],[name]]&amp;"', " &amp; Tableau13[[#This Row],[publiclyAvailable]] &amp; ");"</f>
-        <v>insert into board (id, name, publicly_available) values ('10', 'Board name 10', true);</v>
+        <f>"insert into board (id, name, publicly_available) values ("&amp;Tableau13[[#This Row],[id]]&amp;", '"&amp;Tableau13[[#This Row],[name]]&amp;"', " &amp; Tableau13[[#This Row],[publiclyAvailable]] &amp; ");"</f>
+        <v>insert into board (id, name, publicly_available) values (10, 'Board name 10', true);</v>
       </c>
     </row>
   </sheetData>
@@ -2521,11 +2516,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E54377D5-70D9-4AF6-8B92-D1C9D18CB679}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2611,8 +2606,8 @@
         <v>The content of the topic &lt;1&gt;</v>
       </c>
       <c r="J2" t="str">
-        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('" &amp; B2 &amp; "', '" &amp; C2 &amp; "', '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', '" &amp; Tableau14[[#This Row],[author_id]] &amp; "', " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('1', '1', '2018-12-30 12:56:10', '1', true, 1, 'The title of &lt;1&gt;', 'The content of the topic &lt;1&gt;');</v>
+        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (" &amp; B2 &amp; ", " &amp; C2 &amp; ", '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', " &amp; Tableau14[[#This Row],[author_id]] &amp; ", " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (1, 1, '2018-12-30 12:56:10', 1, true, 1, 'The title of &lt;1&gt;', 'The content of the topic &lt;1&gt;');</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -2653,8 +2648,8 @@
         <v>The content of the topic &lt;2&gt;</v>
       </c>
       <c r="J3" t="str">
-        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('" &amp; B3 &amp; "', '" &amp; C3 &amp; "', '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', '" &amp; Tableau14[[#This Row],[author_id]] &amp; "', " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('2', '2', '2018-12-29 13:57:10', '2', true, 2, 'The title of &lt;2&gt;', 'The content of the topic &lt;2&gt;');</v>
+        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (" &amp; B3 &amp; ", " &amp; C3 &amp; ", '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', " &amp; Tableau14[[#This Row],[author_id]] &amp; ", " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (2, 2, '2018-12-29 13:57:10', 2, true, 2, 'The title of &lt;2&gt;', 'The content of the topic &lt;2&gt;');</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -2695,8 +2690,8 @@
         <v>The content of the topic &lt;3&gt;</v>
       </c>
       <c r="J4" t="str">
-        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('" &amp; B4 &amp; "', '" &amp; C4 &amp; "', '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', '" &amp; Tableau14[[#This Row],[author_id]] &amp; "', " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('3', '3', '2018-12-28 14:58:10', '3', true, 3, 'The title of &lt;3&gt;', 'The content of the topic &lt;3&gt;');</v>
+        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (" &amp; B4 &amp; ", " &amp; C4 &amp; ", '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', " &amp; Tableau14[[#This Row],[author_id]] &amp; ", " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (3, 3, '2018-12-28 14:58:10', 3, true, 3, 'The title of &lt;3&gt;', 'The content of the topic &lt;3&gt;');</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -2737,8 +2732,8 @@
         <v>The content of the topic &lt;4&gt;</v>
       </c>
       <c r="J5" t="str">
-        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('" &amp; B5 &amp; "', '" &amp; C5 &amp; "', '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', '" &amp; Tableau14[[#This Row],[author_id]] &amp; "', " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('4', '4', '2018-12-27 15:59:10', '4', true, 4, 'The title of &lt;4&gt;', 'The content of the topic &lt;4&gt;');</v>
+        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (" &amp; B5 &amp; ", " &amp; C5 &amp; ", '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', " &amp; Tableau14[[#This Row],[author_id]] &amp; ", " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (4, 4, '2018-12-27 15:59:10', 4, true, 4, 'The title of &lt;4&gt;', 'The content of the topic &lt;4&gt;');</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -2779,8 +2774,8 @@
         <v>The content of the topic &lt;5&gt;</v>
       </c>
       <c r="J6" t="str">
-        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('" &amp; B6 &amp; "', '" &amp; C6 &amp; "', '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', '" &amp; Tableau14[[#This Row],[author_id]] &amp; "', " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('5', '5', '2018-12-26 17:00:10', '5', true, 5, 'The title of &lt;5&gt;', 'The content of the topic &lt;5&gt;');</v>
+        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (" &amp; B6 &amp; ", " &amp; C6 &amp; ", '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', " &amp; Tableau14[[#This Row],[author_id]] &amp; ", " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (5, 5, '2018-12-26 17:00:10', 5, true, 5, 'The title of &lt;5&gt;', 'The content of the topic &lt;5&gt;');</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -2821,8 +2816,8 @@
         <v>The content of the topic &lt;6&gt;</v>
       </c>
       <c r="J7" t="str">
-        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('" &amp; B7 &amp; "', '" &amp; C7 &amp; "', '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', '" &amp; Tableau14[[#This Row],[author_id]] &amp; "', " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('6', '6', '2018-12-25 18:01:10', '6', true, 6, 'The title of &lt;6&gt;', 'The content of the topic &lt;6&gt;');</v>
+        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (" &amp; B7 &amp; ", " &amp; C7 &amp; ", '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', " &amp; Tableau14[[#This Row],[author_id]] &amp; ", " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (6, 6, '2018-12-25 18:01:10', 6, true, 6, 'The title of &lt;6&gt;', 'The content of the topic &lt;6&gt;');</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -2863,8 +2858,8 @@
         <v>The content of the topic &lt;7&gt;</v>
       </c>
       <c r="J8" t="str">
-        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('" &amp; B8 &amp; "', '" &amp; C8 &amp; "', '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', '" &amp; Tableau14[[#This Row],[author_id]] &amp; "', " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('7', '7', '2018-12-24 19:02:10', '7', true, 7, 'The title of &lt;7&gt;', 'The content of the topic &lt;7&gt;');</v>
+        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (" &amp; B8 &amp; ", " &amp; C8 &amp; ", '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', " &amp; Tableau14[[#This Row],[author_id]] &amp; ", " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (7, 7, '2018-12-24 19:02:10', 7, true, 7, 'The title of &lt;7&gt;', 'The content of the topic &lt;7&gt;');</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -2905,8 +2900,8 @@
         <v>The content of the topic &lt;8&gt;</v>
       </c>
       <c r="J9" t="str">
-        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('" &amp; B9 &amp; "', '" &amp; C9 &amp; "', '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', '" &amp; Tableau14[[#This Row],[author_id]] &amp; "', " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('8', '8', '2018-12-23 20:03:10', '8', true, 8, 'The title of &lt;8&gt;', 'The content of the topic &lt;8&gt;');</v>
+        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (" &amp; B9 &amp; ", " &amp; C9 &amp; ", '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', " &amp; Tableau14[[#This Row],[author_id]] &amp; ", " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (8, 8, '2018-12-23 20:03:10', 8, true, 8, 'The title of &lt;8&gt;', 'The content of the topic &lt;8&gt;');</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -2947,8 +2942,8 @@
         <v>The content of the topic &lt;9&gt;</v>
       </c>
       <c r="J10" t="str">
-        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('" &amp; B10 &amp; "', '" &amp; C10 &amp; "', '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', '" &amp; Tableau14[[#This Row],[author_id]] &amp; "', " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('9', '9', '2018-12-22 21:04:10', '9', false, 9, 'The title of &lt;9&gt;', 'The content of the topic &lt;9&gt;');</v>
+        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (" &amp; B10 &amp; ", " &amp; C10 &amp; ", '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', " &amp; Tableau14[[#This Row],[author_id]] &amp; ", " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (9, 9, '2018-12-22 21:04:10', 9, false, 9, 'The title of &lt;9&gt;', 'The content of the topic &lt;9&gt;');</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -2989,8 +2984,8 @@
         <v>The content of the topic &lt;10&gt;</v>
       </c>
       <c r="J11" t="str">
-        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('" &amp; B11 &amp; "', '" &amp; C11 &amp; "', '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', '" &amp; Tableau14[[#This Row],[author_id]] &amp; "', " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('10', '10', '2018-12-21 22:05:10', '10', true, 10, 'The title of &lt;10&gt;', 'The content of the topic &lt;10&gt;');</v>
+        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (" &amp; B11 &amp; ", " &amp; C11 &amp; ", '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', " &amp; Tableau14[[#This Row],[author_id]] &amp; ", " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (10, 10, '2018-12-21 22:05:10', 10, true, 10, 'The title of &lt;10&gt;', 'The content of the topic &lt;10&gt;');</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -3031,8 +3026,8 @@
         <v>The content of the topic &lt;11&gt;</v>
       </c>
       <c r="J12" t="str">
-        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('" &amp; B12 &amp; "', '" &amp; C12 &amp; "', '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', '" &amp; Tableau14[[#This Row],[author_id]] &amp; "', " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('11', '1', '2018-12-20 23:06:10', '11', true, 11, 'The title of &lt;11&gt;', 'The content of the topic &lt;11&gt;');</v>
+        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (" &amp; B12 &amp; ", " &amp; C12 &amp; ", '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', " &amp; Tableau14[[#This Row],[author_id]] &amp; ", " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (11, 1, '2018-12-20 23:06:10', 11, true, 11, 'The title of &lt;11&gt;', 'The content of the topic &lt;11&gt;');</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -3073,8 +3068,8 @@
         <v>The content of the topic &lt;12&gt;</v>
       </c>
       <c r="J13" t="str">
-        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('" &amp; B13 &amp; "', '" &amp; C13 &amp; "', '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', '" &amp; Tableau14[[#This Row],[author_id]] &amp; "', " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('12', '2', '2018-12-20 00:07:10', '12', true, 12, 'The title of &lt;12&gt;', 'The content of the topic &lt;12&gt;');</v>
+        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (" &amp; B13 &amp; ", " &amp; C13 &amp; ", '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', " &amp; Tableau14[[#This Row],[author_id]] &amp; ", " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (12, 2, '2018-12-20 00:07:10', 12, true, 12, 'The title of &lt;12&gt;', 'The content of the topic &lt;12&gt;');</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -3115,8 +3110,8 @@
         <v>The content of the topic &lt;13&gt;</v>
       </c>
       <c r="J14" t="str">
-        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('" &amp; B14 &amp; "', '" &amp; C14 &amp; "', '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', '" &amp; Tableau14[[#This Row],[author_id]] &amp; "', " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('13', '3', '2018-12-19 01:08:10', '13', true, 13, 'The title of &lt;13&gt;', 'The content of the topic &lt;13&gt;');</v>
+        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (" &amp; B14 &amp; ", " &amp; C14 &amp; ", '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', " &amp; Tableau14[[#This Row],[author_id]] &amp; ", " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (13, 3, '2018-12-19 01:08:10', 13, true, 13, 'The title of &lt;13&gt;', 'The content of the topic &lt;13&gt;');</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -3157,8 +3152,8 @@
         <v>The content of the topic &lt;14&gt;</v>
       </c>
       <c r="J15" t="str">
-        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('" &amp; B15 &amp; "', '" &amp; C15 &amp; "', '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', '" &amp; Tableau14[[#This Row],[author_id]] &amp; "', " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('14', '4', '2018-12-18 02:09:10', '14', true, 14, 'The title of &lt;14&gt;', 'The content of the topic &lt;14&gt;');</v>
+        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (" &amp; B15 &amp; ", " &amp; C15 &amp; ", '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', " &amp; Tableau14[[#This Row],[author_id]] &amp; ", " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (14, 4, '2018-12-18 02:09:10', 14, true, 14, 'The title of &lt;14&gt;', 'The content of the topic &lt;14&gt;');</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
@@ -3199,8 +3194,8 @@
         <v>The content of the topic &lt;15&gt;</v>
       </c>
       <c r="J16" t="str">
-        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('" &amp; B16 &amp; "', '" &amp; C16 &amp; "', '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', '" &amp; Tableau14[[#This Row],[author_id]] &amp; "', " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('15', '5', '2018-12-17 02:10:10', '15', true, 15, 'The title of &lt;15&gt;', 'The content of the topic &lt;15&gt;');</v>
+        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (" &amp; B16 &amp; ", " &amp; C16 &amp; ", '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', " &amp; Tableau14[[#This Row],[author_id]] &amp; ", " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (15, 5, '2018-12-17 02:10:10', 15, true, 15, 'The title of &lt;15&gt;', 'The content of the topic &lt;15&gt;');</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -3241,8 +3236,8 @@
         <v>The content of the topic &lt;16&gt;</v>
       </c>
       <c r="J17" t="str">
-        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('" &amp; B17 &amp; "', '" &amp; C17 &amp; "', '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', '" &amp; Tableau14[[#This Row],[author_id]] &amp; "', " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('16', '6', '2018-12-16 03:11:10', '16', true, 16, 'The title of &lt;16&gt;', 'The content of the topic &lt;16&gt;');</v>
+        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (" &amp; B17 &amp; ", " &amp; C17 &amp; ", '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', " &amp; Tableau14[[#This Row],[author_id]] &amp; ", " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (16, 6, '2018-12-16 03:11:10', 16, true, 16, 'The title of &lt;16&gt;', 'The content of the topic &lt;16&gt;');</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -3283,8 +3278,8 @@
         <v>The content of the topic &lt;17&gt;</v>
       </c>
       <c r="J18" t="str">
-        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('" &amp; B18 &amp; "', '" &amp; C18 &amp; "', '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', '" &amp; Tableau14[[#This Row],[author_id]] &amp; "', " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('17', '7', '2018-12-15 04:12:10', '17', true, 17, 'The title of &lt;17&gt;', 'The content of the topic &lt;17&gt;');</v>
+        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (" &amp; B18 &amp; ", " &amp; C18 &amp; ", '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', " &amp; Tableau14[[#This Row],[author_id]] &amp; ", " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (17, 7, '2018-12-15 04:12:10', 17, true, 17, 'The title of &lt;17&gt;', 'The content of the topic &lt;17&gt;');</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -3325,8 +3320,8 @@
         <v>The content of the topic &lt;18&gt;</v>
       </c>
       <c r="J19" t="str">
-        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('" &amp; B19 &amp; "', '" &amp; C19 &amp; "', '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', '" &amp; Tableau14[[#This Row],[author_id]] &amp; "', " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('18', '8', '2018-12-14 05:13:10', '18', true, 18, 'The title of &lt;18&gt;', 'The content of the topic &lt;18&gt;');</v>
+        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (" &amp; B19 &amp; ", " &amp; C19 &amp; ", '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', " &amp; Tableau14[[#This Row],[author_id]] &amp; ", " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (18, 8, '2018-12-14 05:13:10', 18, true, 18, 'The title of &lt;18&gt;', 'The content of the topic &lt;18&gt;');</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -3367,8 +3362,8 @@
         <v>The content of the topic &lt;19&gt;</v>
       </c>
       <c r="J20" t="str">
-        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('" &amp; B20 &amp; "', '" &amp; C20 &amp; "', '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', '" &amp; Tableau14[[#This Row],[author_id]] &amp; "', " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('19', '9', '2018-12-13 06:14:10', '19', false, 19, 'The title of &lt;19&gt;', 'The content of the topic &lt;19&gt;');</v>
+        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (" &amp; B20 &amp; ", " &amp; C20 &amp; ", '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', " &amp; Tableau14[[#This Row],[author_id]] &amp; ", " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (19, 9, '2018-12-13 06:14:10', 19, false, 19, 'The title of &lt;19&gt;', 'The content of the topic &lt;19&gt;');</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
@@ -3409,8 +3404,8 @@
         <v>The content of the topic &lt;20&gt;</v>
       </c>
       <c r="J21" t="str">
-        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('" &amp; B21 &amp; "', '" &amp; C21 &amp; "', '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', '" &amp; Tableau14[[#This Row],[author_id]] &amp; "', " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('20', '10', '2018-12-12 07:15:10', '20', true, 20, 'The title of &lt;20&gt;', 'The content of the topic &lt;20&gt;');</v>
+        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (" &amp; B21 &amp; ", " &amp; C21 &amp; ", '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', " &amp; Tableau14[[#This Row],[author_id]] &amp; ", " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (20, 10, '2018-12-12 07:15:10', 20, true, 20, 'The title of &lt;20&gt;', 'The content of the topic &lt;20&gt;');</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -3451,8 +3446,8 @@
         <v>The content of the topic &lt;21&gt;</v>
       </c>
       <c r="J22" t="str">
-        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('" &amp; B22 &amp; "', '" &amp; C22 &amp; "', '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', '" &amp; Tableau14[[#This Row],[author_id]] &amp; "', " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('21', '1', '2018-12-11 08:16:10', '21', true, 21, 'The title of &lt;21&gt;', 'The content of the topic &lt;21&gt;');</v>
+        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (" &amp; B22 &amp; ", " &amp; C22 &amp; ", '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', " &amp; Tableau14[[#This Row],[author_id]] &amp; ", " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (21, 1, '2018-12-11 08:16:10', 21, true, 21, 'The title of &lt;21&gt;', 'The content of the topic &lt;21&gt;');</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -3493,8 +3488,8 @@
         <v>The content of the topic &lt;22&gt;</v>
       </c>
       <c r="J23" t="str">
-        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('" &amp; B23 &amp; "', '" &amp; C23 &amp; "', '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', '" &amp; Tableau14[[#This Row],[author_id]] &amp; "', " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('22', '2', '2018-12-09 10:17:10', '22', true, 22, 'The title of &lt;22&gt;', 'The content of the topic &lt;22&gt;');</v>
+        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (" &amp; B23 &amp; ", " &amp; C23 &amp; ", '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', " &amp; Tableau14[[#This Row],[author_id]] &amp; ", " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (22, 2, '2018-12-09 10:17:10', 22, true, 22, 'The title of &lt;22&gt;', 'The content of the topic &lt;22&gt;');</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
@@ -3535,8 +3530,8 @@
         <v>The content of the topic &lt;23&gt;</v>
       </c>
       <c r="J24" t="str">
-        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('" &amp; B24 &amp; "', '" &amp; C24 &amp; "', '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', '" &amp; Tableau14[[#This Row],[author_id]] &amp; "', " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('23', '3', '2018-12-08 11:18:10', '23', true, 23, 'The title of &lt;23&gt;', 'The content of the topic &lt;23&gt;');</v>
+        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (" &amp; B24 &amp; ", " &amp; C24 &amp; ", '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', " &amp; Tableau14[[#This Row],[author_id]] &amp; ", " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (23, 3, '2018-12-08 11:18:10', 23, true, 23, 'The title of &lt;23&gt;', 'The content of the topic &lt;23&gt;');</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
@@ -3577,8 +3572,8 @@
         <v>The content of the topic &lt;24&gt;</v>
       </c>
       <c r="J25" t="str">
-        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('" &amp; B25 &amp; "', '" &amp; C25 &amp; "', '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', '" &amp; Tableau14[[#This Row],[author_id]] &amp; "', " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('24', '4', '2018-12-07 12:19:10', '24', true, 24, 'The title of &lt;24&gt;', 'The content of the topic &lt;24&gt;');</v>
+        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (" &amp; B25 &amp; ", " &amp; C25 &amp; ", '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', " &amp; Tableau14[[#This Row],[author_id]] &amp; ", " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (24, 4, '2018-12-07 12:19:10', 24, true, 24, 'The title of &lt;24&gt;', 'The content of the topic &lt;24&gt;');</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
@@ -3619,8 +3614,8 @@
         <v>The content of the topic &lt;25&gt;</v>
       </c>
       <c r="J26" t="str">
-        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('" &amp; B26 &amp; "', '" &amp; C26 &amp; "', '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', '" &amp; Tableau14[[#This Row],[author_id]] &amp; "', " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('25', '5', '2018-12-06 13:20:10', '25', true, 25, 'The title of &lt;25&gt;', 'The content of the topic &lt;25&gt;');</v>
+        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (" &amp; B26 &amp; ", " &amp; C26 &amp; ", '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', " &amp; Tableau14[[#This Row],[author_id]] &amp; ", " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (25, 5, '2018-12-06 13:20:10', 25, true, 25, 'The title of &lt;25&gt;', 'The content of the topic &lt;25&gt;');</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
@@ -3661,8 +3656,8 @@
         <v>The content of the topic &lt;26&gt;</v>
       </c>
       <c r="J27" t="str">
-        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('" &amp; B27 &amp; "', '" &amp; C27 &amp; "', '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', '" &amp; Tableau14[[#This Row],[author_id]] &amp; "', " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('26', '6', '2018-12-05 14:21:10', '26', true, 26, 'The title of &lt;26&gt;', 'The content of the topic &lt;26&gt;');</v>
+        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (" &amp; B27 &amp; ", " &amp; C27 &amp; ", '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', " &amp; Tableau14[[#This Row],[author_id]] &amp; ", " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (26, 6, '2018-12-05 14:21:10', 26, true, 26, 'The title of &lt;26&gt;', 'The content of the topic &lt;26&gt;');</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
@@ -3703,8 +3698,8 @@
         <v>The content of the topic &lt;27&gt;</v>
       </c>
       <c r="J28" t="str">
-        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('" &amp; B28 &amp; "', '" &amp; C28 &amp; "', '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', '" &amp; Tableau14[[#This Row],[author_id]] &amp; "', " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('27', '7', '2018-12-04 15:22:10', '27', true, 27, 'The title of &lt;27&gt;', 'The content of the topic &lt;27&gt;');</v>
+        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (" &amp; B28 &amp; ", " &amp; C28 &amp; ", '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', " &amp; Tableau14[[#This Row],[author_id]] &amp; ", " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (27, 7, '2018-12-04 15:22:10', 27, true, 27, 'The title of &lt;27&gt;', 'The content of the topic &lt;27&gt;');</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
@@ -3745,8 +3740,8 @@
         <v>The content of the topic &lt;28&gt;</v>
       </c>
       <c r="J29" t="str">
-        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('" &amp; B29 &amp; "', '" &amp; C29 &amp; "', '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', '" &amp; Tableau14[[#This Row],[author_id]] &amp; "', " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('28', '8', '2018-12-03 16:23:10', '28', true, 28, 'The title of &lt;28&gt;', 'The content of the topic &lt;28&gt;');</v>
+        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (" &amp; B29 &amp; ", " &amp; C29 &amp; ", '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', " &amp; Tableau14[[#This Row],[author_id]] &amp; ", " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (28, 8, '2018-12-03 16:23:10', 28, true, 28, 'The title of &lt;28&gt;', 'The content of the topic &lt;28&gt;');</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
@@ -3787,8 +3782,8 @@
         <v>The content of the topic &lt;29&gt;</v>
       </c>
       <c r="J30" t="str">
-        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('" &amp; B30 &amp; "', '" &amp; C30 &amp; "', '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', '" &amp; Tableau14[[#This Row],[author_id]] &amp; "', " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('29', '9', '2018-12-02 17:24:10', '29', false, 29, 'The title of &lt;29&gt;', 'The content of the topic &lt;29&gt;');</v>
+        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (" &amp; B30 &amp; ", " &amp; C30 &amp; ", '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', " &amp; Tableau14[[#This Row],[author_id]] &amp; ", " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (29, 9, '2018-12-02 17:24:10', 29, false, 29, 'The title of &lt;29&gt;', 'The content of the topic &lt;29&gt;');</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
@@ -3829,8 +3824,8 @@
         <v>The content of the topic &lt;30&gt;</v>
       </c>
       <c r="J31" t="str">
-        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('" &amp; B31 &amp; "', '" &amp; C31 &amp; "', '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', '" &amp; Tableau14[[#This Row],[author_id]] &amp; "', " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('30', '10', '2018-12-01 18:25:10', '30', true, 30, 'The title of &lt;30&gt;', 'The content of the topic &lt;30&gt;');</v>
+        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (" &amp; B31 &amp; ", " &amp; C31 &amp; ", '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', " &amp; Tableau14[[#This Row],[author_id]] &amp; ", " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (30, 10, '2018-12-01 18:25:10', 30, true, 30, 'The title of &lt;30&gt;', 'The content of the topic &lt;30&gt;');</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
@@ -3871,8 +3866,8 @@
         <v>The content of the topic &lt;31&gt;</v>
       </c>
       <c r="J32" t="str">
-        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('" &amp; B32 &amp; "', '" &amp; C32 &amp; "', '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', '" &amp; Tableau14[[#This Row],[author_id]] &amp; "', " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('31', '1', '2018-11-30 19:26:10', '31', true, 31, 'The title of &lt;31&gt;', 'The content of the topic &lt;31&gt;');</v>
+        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (" &amp; B32 &amp; ", " &amp; C32 &amp; ", '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', " &amp; Tableau14[[#This Row],[author_id]] &amp; ", " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (31, 1, '2018-11-30 19:26:10', 31, true, 31, 'The title of &lt;31&gt;', 'The content of the topic &lt;31&gt;');</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
@@ -3913,8 +3908,8 @@
         <v>The content of the topic &lt;32&gt;</v>
       </c>
       <c r="J33" t="str">
-        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('" &amp; B33 &amp; "', '" &amp; C33 &amp; "', '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', '" &amp; Tableau14[[#This Row],[author_id]] &amp; "', " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('32', '2', '2018-11-29 20:27:10', '32', true, 32, 'The title of &lt;32&gt;', 'The content of the topic &lt;32&gt;');</v>
+        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (" &amp; B33 &amp; ", " &amp; C33 &amp; ", '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', " &amp; Tableau14[[#This Row],[author_id]] &amp; ", " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (32, 2, '2018-11-29 20:27:10', 32, true, 32, 'The title of &lt;32&gt;', 'The content of the topic &lt;32&gt;');</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
@@ -3955,8 +3950,8 @@
         <v>The content of the topic &lt;33&gt;</v>
       </c>
       <c r="J34" t="str">
-        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('" &amp; B34 &amp; "', '" &amp; C34 &amp; "', '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', '" &amp; Tableau14[[#This Row],[author_id]] &amp; "', " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('33', '3', '2018-11-28 21:28:10', '33', true, 33, 'The title of &lt;33&gt;', 'The content of the topic &lt;33&gt;');</v>
+        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (" &amp; B34 &amp; ", " &amp; C34 &amp; ", '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', " &amp; Tableau14[[#This Row],[author_id]] &amp; ", " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (33, 3, '2018-11-28 21:28:10', 33, true, 33, 'The title of &lt;33&gt;', 'The content of the topic &lt;33&gt;');</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
@@ -3997,8 +3992,8 @@
         <v>The content of the topic &lt;34&gt;</v>
       </c>
       <c r="J35" t="str">
-        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('" &amp; B35 &amp; "', '" &amp; C35 &amp; "', '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', '" &amp; Tableau14[[#This Row],[author_id]] &amp; "', " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('34', '4', '2018-11-27 22:29:10', '34', true, 34, 'The title of &lt;34&gt;', 'The content of the topic &lt;34&gt;');</v>
+        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (" &amp; B35 &amp; ", " &amp; C35 &amp; ", '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', " &amp; Tableau14[[#This Row],[author_id]] &amp; ", " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (34, 4, '2018-11-27 22:29:10', 34, true, 34, 'The title of &lt;34&gt;', 'The content of the topic &lt;34&gt;');</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
@@ -4039,8 +4034,8 @@
         <v>The content of the topic &lt;35&gt;</v>
       </c>
       <c r="J36" t="str">
-        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('" &amp; B36 &amp; "', '" &amp; C36 &amp; "', '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', '" &amp; Tableau14[[#This Row],[author_id]] &amp; "', " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('35', '5', '2018-11-26 23:30:10', '35', true, 35, 'The title of &lt;35&gt;', 'The content of the topic &lt;35&gt;');</v>
+        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (" &amp; B36 &amp; ", " &amp; C36 &amp; ", '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', " &amp; Tableau14[[#This Row],[author_id]] &amp; ", " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (35, 5, '2018-11-26 23:30:10', 35, true, 35, 'The title of &lt;35&gt;', 'The content of the topic &lt;35&gt;');</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
@@ -4081,8 +4076,8 @@
         <v>The content of the topic &lt;36&gt;</v>
       </c>
       <c r="J37" t="str">
-        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('" &amp; B37 &amp; "', '" &amp; C37 &amp; "', '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', '" &amp; Tableau14[[#This Row],[author_id]] &amp; "', " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('36', '6', '2018-11-26 00:31:10', '36', true, 36, 'The title of &lt;36&gt;', 'The content of the topic &lt;36&gt;');</v>
+        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (" &amp; B37 &amp; ", " &amp; C37 &amp; ", '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', " &amp; Tableau14[[#This Row],[author_id]] &amp; ", " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (36, 6, '2018-11-26 00:31:10', 36, true, 36, 'The title of &lt;36&gt;', 'The content of the topic &lt;36&gt;');</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
@@ -4123,8 +4118,8 @@
         <v>The content of the topic &lt;37&gt;</v>
       </c>
       <c r="J38" t="str">
-        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('" &amp; B38 &amp; "', '" &amp; C38 &amp; "', '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', '" &amp; Tableau14[[#This Row],[author_id]] &amp; "', " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('37', '7', '2018-11-25 01:32:10', '37', true, 37, 'The title of &lt;37&gt;', 'The content of the topic &lt;37&gt;');</v>
+        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (" &amp; B38 &amp; ", " &amp; C38 &amp; ", '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', " &amp; Tableau14[[#This Row],[author_id]] &amp; ", " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (37, 7, '2018-11-25 01:32:10', 37, true, 37, 'The title of &lt;37&gt;', 'The content of the topic &lt;37&gt;');</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
@@ -4165,8 +4160,8 @@
         <v>The content of the topic &lt;38&gt;</v>
       </c>
       <c r="J39" t="str">
-        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('" &amp; B39 &amp; "', '" &amp; C39 &amp; "', '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', '" &amp; Tableau14[[#This Row],[author_id]] &amp; "', " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('38', '8', '2018-11-24 02:33:10', '38', true, 38, 'The title of &lt;38&gt;', 'The content of the topic &lt;38&gt;');</v>
+        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (" &amp; B39 &amp; ", " &amp; C39 &amp; ", '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', " &amp; Tableau14[[#This Row],[author_id]] &amp; ", " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (38, 8, '2018-11-24 02:33:10', 38, true, 38, 'The title of &lt;38&gt;', 'The content of the topic &lt;38&gt;');</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
@@ -4207,8 +4202,8 @@
         <v>The content of the topic &lt;39&gt;</v>
       </c>
       <c r="J40" t="str">
-        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('" &amp; B40 &amp; "', '" &amp; C40 &amp; "', '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', '" &amp; Tableau14[[#This Row],[author_id]] &amp; "', " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('39', '9', '2018-11-23 03:34:10', '39', false, 39, 'The title of &lt;39&gt;', 'The content of the topic &lt;39&gt;');</v>
+        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (" &amp; B40 &amp; ", " &amp; C40 &amp; ", '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', " &amp; Tableau14[[#This Row],[author_id]] &amp; ", " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (39, 9, '2018-11-23 03:34:10', 39, false, 39, 'The title of &lt;39&gt;', 'The content of the topic &lt;39&gt;');</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
@@ -4249,8 +4244,8 @@
         <v>The content of the topic &lt;40&gt;</v>
       </c>
       <c r="J41" t="str">
-        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('" &amp; B41 &amp; "', '" &amp; C41 &amp; "', '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', '" &amp; Tableau14[[#This Row],[author_id]] &amp; "', " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('40', '10', '2018-11-22 04:35:10', '40', true, 40, 'The title of &lt;40&gt;', 'The content of the topic &lt;40&gt;');</v>
+        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (" &amp; B41 &amp; ", " &amp; C41 &amp; ", '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', " &amp; Tableau14[[#This Row],[author_id]] &amp; ", " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (40, 10, '2018-11-22 04:35:10', 40, true, 40, 'The title of &lt;40&gt;', 'The content of the topic &lt;40&gt;');</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
@@ -4291,8 +4286,8 @@
         <v>The content of the topic &lt;41&gt;</v>
       </c>
       <c r="J42" t="str">
-        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('" &amp; B42 &amp; "', '" &amp; C42 &amp; "', '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', '" &amp; Tableau14[[#This Row],[author_id]] &amp; "', " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('41', '1', '2018-11-21 05:36:10', '41', true, 41, 'The title of &lt;41&gt;', 'The content of the topic &lt;41&gt;');</v>
+        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (" &amp; B42 &amp; ", " &amp; C42 &amp; ", '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', " &amp; Tableau14[[#This Row],[author_id]] &amp; ", " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (41, 1, '2018-11-21 05:36:10', 41, true, 41, 'The title of &lt;41&gt;', 'The content of the topic &lt;41&gt;');</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
@@ -4333,8 +4328,8 @@
         <v>The content of the topic &lt;42&gt;</v>
       </c>
       <c r="J43" t="str">
-        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('" &amp; B43 &amp; "', '" &amp; C43 &amp; "', '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', '" &amp; Tableau14[[#This Row],[author_id]] &amp; "', " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('42', '2', '2018-11-20 06:37:10', '42', true, 42, 'The title of &lt;42&gt;', 'The content of the topic &lt;42&gt;');</v>
+        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (" &amp; B43 &amp; ", " &amp; C43 &amp; ", '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', " &amp; Tableau14[[#This Row],[author_id]] &amp; ", " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (42, 2, '2018-11-20 06:37:10', 42, true, 42, 'The title of &lt;42&gt;', 'The content of the topic &lt;42&gt;');</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
@@ -4375,8 +4370,8 @@
         <v>The content of the topic &lt;43&gt;</v>
       </c>
       <c r="J44" t="str">
-        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('" &amp; B44 &amp; "', '" &amp; C44 &amp; "', '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', '" &amp; Tableau14[[#This Row],[author_id]] &amp; "', " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('43', '3', '2018-11-19 07:38:10', '43', true, 43, 'The title of &lt;43&gt;', 'The content of the topic &lt;43&gt;');</v>
+        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (" &amp; B44 &amp; ", " &amp; C44 &amp; ", '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', " &amp; Tableau14[[#This Row],[author_id]] &amp; ", " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (43, 3, '2018-11-19 07:38:10', 43, true, 43, 'The title of &lt;43&gt;', 'The content of the topic &lt;43&gt;');</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
@@ -4417,8 +4412,8 @@
         <v>The content of the topic &lt;44&gt;</v>
       </c>
       <c r="J45" t="str">
-        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('" &amp; B45 &amp; "', '" &amp; C45 &amp; "', '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', '" &amp; Tableau14[[#This Row],[author_id]] &amp; "', " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('44', '4', '2018-11-18 08:39:10', '44', true, 44, 'The title of &lt;44&gt;', 'The content of the topic &lt;44&gt;');</v>
+        <f>"insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (" &amp; B45 &amp; ", " &amp; C45 &amp; ", '" &amp; TEXT(Tableau14[[#This Row],[date]], "AAAA-MM-JJ HH:MM:SS") &amp; "', " &amp; Tableau14[[#This Row],[author_id]] &amp; ", " &amp; Tableau14[[#This Row],[publiclyAvailable]] &amp; ", " &amp; Tableau14[[#This Row],[nbPosts]] &amp; ", '" &amp; Tableau14[[#This Row],[title]] &amp; "', '" &amp; Tableau14[[#This Row],[content]] &amp; "');"</f>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (44, 4, '2018-11-18 08:39:10', 44, true, 44, 'The title of &lt;44&gt;', 'The content of the topic &lt;44&gt;');</v>
       </c>
     </row>
   </sheetData>
@@ -4431,11 +4426,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{807A625F-0616-4062-970A-980DBE24F189}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I321"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D321"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16648,11 +16643,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79C37643-EB7B-4ACB-AFCB-2C4BB49D263A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I529"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A262" workbookViewId="0">
+      <selection activeCell="F273" sqref="F273"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16709,7 +16704,7 @@
       </c>
       <c r="F2" s="5" t="str">
         <f ca="1">IF( OR(F1="commit;",F1=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('1', 'Name 1', null, 'name.1@graphql-java.com', 'ADMIN'); </v>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (1, 'Name 1', null, 'name.1@graphql-java.com', 'ADMIN'); </v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -16735,7 +16730,7 @@
       </c>
       <c r="F3" s="5" t="str">
         <f ca="1">IF( OR(F2="commit;",F2=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('2', 'Name 2', 'Alias of Name 2', 'name.2@graphql-java.com', 'MODERATOR'); </v>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (2, 'Name 2', 'Alias of Name 2', 'name.2@graphql-java.com', 'MODERATOR'); </v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -16761,7 +16756,7 @@
       </c>
       <c r="F4" s="5" t="str">
         <f ca="1">IF( OR(F3="commit;",F3=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('3', 'Name 3', null, 'name.3@graphql-java.com', 'STANDARD'); </v>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (3, 'Name 3', null, 'name.3@graphql-java.com', 'STANDARD'); </v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -16787,14 +16782,14 @@
       </c>
       <c r="F5" s="5" t="str">
         <f ca="1">IF( OR(F4="commit;",F4=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('4', 'Name 4', 'Alias of Name 4', 'name.4@graphql-java.com', 'ADMIN'); </v>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (4, 'Name 4', 'Alias of Name 4', 'name.4@graphql-java.com', 'ADMIN'); </v>
       </c>
       <c r="H5" t="s">
         <v>66</v>
       </c>
       <c r="I5" t="str">
         <f ca="1">INDIRECT(H5)</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('1', 'Name 1', null, 'name.1@graphql-java.com', 'ADMIN'); </v>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (1, 'Name 1', null, 'name.1@graphql-java.com', 'ADMIN'); </v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -16820,14 +16815,14 @@
       </c>
       <c r="F6" s="5" t="str">
         <f ca="1">IF( OR(F5="commit;",F5=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('5', 'Name 5', null, 'name.5@graphql-java.com', 'MODERATOR'); </v>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (5, 'Name 5', null, 'name.5@graphql-java.com', 'MODERATOR'); </v>
       </c>
       <c r="H6" t="s">
         <v>67</v>
       </c>
       <c r="I6" t="str">
         <f t="shared" ref="I6:I10" ca="1" si="1">INDIRECT(H6)</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('2', 'Name 2', 'Alias of Name 2', 'name.2@graphql-java.com', 'MODERATOR'); </v>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (2, 'Name 2', 'Alias of Name 2', 'name.2@graphql-java.com', 'MODERATOR'); </v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -16853,14 +16848,14 @@
       </c>
       <c r="F7" s="5" t="str">
         <f ca="1">IF( OR(F6="commit;",F6=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('6', 'Name 6', 'Alias of Name 6', 'name.6@graphql-java.com', 'STANDARD'); </v>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (6, 'Name 6', 'Alias of Name 6', 'name.6@graphql-java.com', 'STANDARD'); </v>
       </c>
       <c r="H7" t="s">
         <v>68</v>
       </c>
       <c r="I7" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('3', 'Name 3', null, 'name.3@graphql-java.com', 'STANDARD'); </v>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (3, 'Name 3', null, 'name.3@graphql-java.com', 'STANDARD'); </v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -16886,14 +16881,14 @@
       </c>
       <c r="F8" s="5" t="str">
         <f ca="1">IF( OR(F7="commit;",F7=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('7', 'Name 7', null, 'name.7@graphql-java.com', 'ADMIN'); </v>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (7, 'Name 7', null, 'name.7@graphql-java.com', 'ADMIN'); </v>
       </c>
       <c r="H8" t="s">
         <v>69</v>
       </c>
       <c r="I8" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('4', 'Name 4', 'Alias of Name 4', 'name.4@graphql-java.com', 'ADMIN'); </v>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (4, 'Name 4', 'Alias of Name 4', 'name.4@graphql-java.com', 'ADMIN'); </v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -16919,14 +16914,14 @@
       </c>
       <c r="F9" s="5" t="str">
         <f ca="1">IF( OR(F8="commit;",F8=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('8', 'Name 8', 'Alias of Name 8', 'name.8@graphql-java.com', 'MODERATOR'); </v>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (8, 'Name 8', 'Alias of Name 8', 'name.8@graphql-java.com', 'MODERATOR'); </v>
       </c>
       <c r="H9" t="s">
         <v>70</v>
       </c>
       <c r="I9" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('5', 'Name 5', null, 'name.5@graphql-java.com', 'MODERATOR'); </v>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (5, 'Name 5', null, 'name.5@graphql-java.com', 'MODERATOR'); </v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -16952,14 +16947,14 @@
       </c>
       <c r="F10" s="5" t="str">
         <f ca="1">IF( OR(F9="commit;",F9=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('9', 'Name 9', null, 'name.9@graphql-java.com', 'STANDARD'); </v>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (9, 'Name 9', null, 'name.9@graphql-java.com', 'STANDARD'); </v>
       </c>
       <c r="H10" t="s">
         <v>71</v>
       </c>
       <c r="I10" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('6', 'Name 6', 'Alias of Name 6', 'name.6@graphql-java.com', 'STANDARD'); </v>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (6, 'Name 6', 'Alias of Name 6', 'name.6@graphql-java.com', 'STANDARD'); </v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -16985,7 +16980,7 @@
       </c>
       <c r="F11" s="5" t="str">
         <f ca="1">IF( OR(F10="commit;",F10=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('10', 'Name 10', 'Alias of Name 10', 'name.10@graphql-java.com', 'ADMIN'); </v>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (10, 'Name 10', 'Alias of Name 10', 'name.10@graphql-java.com', 'ADMIN'); </v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -17011,7 +17006,7 @@
       </c>
       <c r="F12" s="5" t="str">
         <f ca="1">IF( OR(F11="commit;",F11=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('11', 'Name 11', null, 'name.11@graphql-java.com', 'MODERATOR'); </v>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (11, 'Name 11', null, 'name.11@graphql-java.com', 'MODERATOR'); </v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -17037,7 +17032,7 @@
       </c>
       <c r="F13" s="5" t="str">
         <f ca="1">IF( OR(F12="commit;",F12=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('12', 'Name 12', 'Alias of Name 12', 'name.12@graphql-java.com', 'STANDARD'); </v>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (12, 'Name 12', 'Alias of Name 12', 'name.12@graphql-java.com', 'STANDARD'); </v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -17063,7 +17058,7 @@
       </c>
       <c r="F14" s="5" t="str">
         <f ca="1">IF( OR(F13="commit;",F13=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('13', 'Name 13', null, 'name.13@graphql-java.com', 'ADMIN'); </v>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (13, 'Name 13', null, 'name.13@graphql-java.com', 'ADMIN'); </v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -17089,7 +17084,7 @@
       </c>
       <c r="F15" s="5" t="str">
         <f ca="1">IF( OR(F14="commit;",F14=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('14', 'Name 14', 'Alias of Name 14', 'name.14@graphql-java.com', 'MODERATOR'); </v>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (14, 'Name 14', 'Alias of Name 14', 'name.14@graphql-java.com', 'MODERATOR'); </v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -17115,7 +17110,7 @@
       </c>
       <c r="F16" s="5" t="str">
         <f ca="1">IF( OR(F15="commit;",F15=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('15', 'Name 15', null, 'name.15@graphql-java.com', 'STANDARD'); </v>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (15, 'Name 15', null, 'name.15@graphql-java.com', 'STANDARD'); </v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -17141,7 +17136,7 @@
       </c>
       <c r="F17" s="5" t="str">
         <f ca="1">IF( OR(F16="commit;",F16=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('16', 'Name 16', 'Alias of Name 16', 'name.16@graphql-java.com', 'ADMIN'); </v>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (16, 'Name 16', 'Alias of Name 16', 'name.16@graphql-java.com', 'ADMIN'); </v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -17167,7 +17162,7 @@
       </c>
       <c r="F18" s="5" t="str">
         <f ca="1">IF( OR(F17="commit;",F17=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('17', 'Name 17', null, 'name.17@graphql-java.com', 'MODERATOR'); </v>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (17, 'Name 17', null, 'name.17@graphql-java.com', 'MODERATOR'); </v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -17193,7 +17188,7 @@
       </c>
       <c r="F19" s="5" t="str">
         <f ca="1">IF( OR(F18="commit;",F18=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('18', 'Name 18', 'Alias of Name 18', 'name.18@graphql-java.com', 'STANDARD'); </v>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (18, 'Name 18', 'Alias of Name 18', 'name.18@graphql-java.com', 'STANDARD'); </v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -17219,7 +17214,7 @@
       </c>
       <c r="F20" s="5" t="str">
         <f ca="1">IF( OR(F19="commit;",F19=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('19', 'Name 19', null, 'name.19@graphql-java.com', 'ADMIN'); </v>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (19, 'Name 19', null, 'name.19@graphql-java.com', 'ADMIN'); </v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -17245,7 +17240,7 @@
       </c>
       <c r="F21" s="5" t="str">
         <f ca="1">IF( OR(F20="commit;",F20=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('20', 'Name 20', 'Alias of Name 20', 'name.20@graphql-java.com', 'MODERATOR'); </v>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (20, 'Name 20', 'Alias of Name 20', 'name.20@graphql-java.com', 'MODERATOR'); </v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -17271,7 +17266,7 @@
       </c>
       <c r="F22" s="5" t="str">
         <f ca="1">IF( OR(F21="commit;",F21=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('21', 'Name 21', null, 'name.21@graphql-java.com', 'STANDARD'); </v>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (21, 'Name 21', null, 'name.21@graphql-java.com', 'STANDARD'); </v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -17297,7 +17292,7 @@
       </c>
       <c r="F23" s="5" t="str">
         <f ca="1">IF( OR(F22="commit;",F22=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('22', 'Name 22', 'Alias of Name 22', 'name.22@graphql-java.com', 'ADMIN'); </v>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (22, 'Name 22', 'Alias of Name 22', 'name.22@graphql-java.com', 'ADMIN'); </v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -17323,7 +17318,7 @@
       </c>
       <c r="F24" s="5" t="str">
         <f ca="1">IF( OR(F23="commit;",F23=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('23', 'Name 23', null, 'name.23@graphql-java.com', 'MODERATOR'); </v>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (23, 'Name 23', null, 'name.23@graphql-java.com', 'MODERATOR'); </v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -17349,7 +17344,7 @@
       </c>
       <c r="F25" s="5" t="str">
         <f ca="1">IF( OR(F24="commit;",F24=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('24', 'Name 24', 'Alias of Name 24', 'name.24@graphql-java.com', 'STANDARD'); </v>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (24, 'Name 24', 'Alias of Name 24', 'name.24@graphql-java.com', 'STANDARD'); </v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -17375,7 +17370,7 @@
       </c>
       <c r="F26" s="5" t="str">
         <f ca="1">IF( OR(F25="commit;",F25=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('25', 'Name 25', null, 'name.25@graphql-java.com', 'ADMIN'); </v>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (25, 'Name 25', null, 'name.25@graphql-java.com', 'ADMIN'); </v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -17401,7 +17396,7 @@
       </c>
       <c r="F27" s="5" t="str">
         <f ca="1">IF( OR(F26="commit;",F26=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('26', 'Name 26', 'Alias of Name 26', 'name.26@graphql-java.com', 'MODERATOR'); </v>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (26, 'Name 26', 'Alias of Name 26', 'name.26@graphql-java.com', 'MODERATOR'); </v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -17427,7 +17422,7 @@
       </c>
       <c r="F28" s="5" t="str">
         <f ca="1">IF( OR(F27="commit;",F27=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('27', 'Name 27', null, 'name.27@graphql-java.com', 'STANDARD'); </v>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (27, 'Name 27', null, 'name.27@graphql-java.com', 'STANDARD'); </v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -17453,7 +17448,7 @@
       </c>
       <c r="F29" s="5" t="str">
         <f ca="1">IF( OR(F28="commit;",F28=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('28', 'Name 28', 'Alias of Name 28', 'name.28@graphql-java.com', 'ADMIN'); </v>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (28, 'Name 28', 'Alias of Name 28', 'name.28@graphql-java.com', 'ADMIN'); </v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -17479,7 +17474,7 @@
       </c>
       <c r="F30" s="5" t="str">
         <f ca="1">IF( OR(F29="commit;",F29=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('29', 'Name 29', null, 'name.29@graphql-java.com', 'MODERATOR'); </v>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (29, 'Name 29', null, 'name.29@graphql-java.com', 'MODERATOR'); </v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -17505,7 +17500,7 @@
       </c>
       <c r="F31" s="5" t="str">
         <f ca="1">IF( OR(F30="commit;",F30=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('30', 'Name 30', 'Alias of Name 30', 'name.30@graphql-java.com', 'STANDARD'); </v>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (30, 'Name 30', 'Alias of Name 30', 'name.30@graphql-java.com', 'STANDARD'); </v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -17531,7 +17526,7 @@
       </c>
       <c r="F32" s="5" t="str">
         <f ca="1">IF( OR(F31="commit;",F31=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('31', 'Name 31', null, 'name.31@graphql-java.com', 'ADMIN'); </v>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (31, 'Name 31', null, 'name.31@graphql-java.com', 'ADMIN'); </v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -17557,7 +17552,7 @@
       </c>
       <c r="F33" s="5" t="str">
         <f ca="1">IF( OR(F32="commit;",F32=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('32', 'Name 32', 'Alias of Name 32', 'name.32@graphql-java.com', 'MODERATOR'); </v>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (32, 'Name 32', 'Alias of Name 32', 'name.32@graphql-java.com', 'MODERATOR'); </v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -17583,7 +17578,7 @@
       </c>
       <c r="F34" s="5" t="str">
         <f ca="1">IF( OR(F33="commit;",F33=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('33', 'Name 33', null, 'name.33@graphql-java.com', 'STANDARD'); </v>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (33, 'Name 33', null, 'name.33@graphql-java.com', 'STANDARD'); </v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -17609,7 +17604,7 @@
       </c>
       <c r="F35" s="5" t="str">
         <f ca="1">IF( OR(F34="commit;",F34=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('34', 'Name 34', 'Alias of Name 34', 'name.34@graphql-java.com', 'ADMIN'); </v>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (34, 'Name 34', 'Alias of Name 34', 'name.34@graphql-java.com', 'ADMIN'); </v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -17635,7 +17630,7 @@
       </c>
       <c r="F36" s="5" t="str">
         <f ca="1">IF( OR(F35="commit;",F35=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('35', 'Name 35', null, 'name.35@graphql-java.com', 'MODERATOR'); </v>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (35, 'Name 35', null, 'name.35@graphql-java.com', 'MODERATOR'); </v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -17661,7 +17656,7 @@
       </c>
       <c r="F37" s="5" t="str">
         <f ca="1">IF( OR(F36="commit;",F36=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('36', 'Name 36', 'Alias of Name 36', 'name.36@graphql-java.com', 'STANDARD'); </v>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (36, 'Name 36', 'Alias of Name 36', 'name.36@graphql-java.com', 'STANDARD'); </v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -17687,7 +17682,7 @@
       </c>
       <c r="F38" s="5" t="str">
         <f ca="1">IF( OR(F37="commit;",F37=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('37', 'Name 37', null, 'name.37@graphql-java.com', 'ADMIN'); </v>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (37, 'Name 37', null, 'name.37@graphql-java.com', 'ADMIN'); </v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -17713,7 +17708,7 @@
       </c>
       <c r="F39" s="5" t="str">
         <f ca="1">IF( OR(F38="commit;",F38=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('38', 'Name 38', 'Alias of Name 38', 'name.38@graphql-java.com', 'MODERATOR'); </v>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (38, 'Name 38', 'Alias of Name 38', 'name.38@graphql-java.com', 'MODERATOR'); </v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -17739,7 +17734,7 @@
       </c>
       <c r="F40" s="5" t="str">
         <f ca="1">IF( OR(F39="commit;",F39=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('39', 'Name 39', null, 'name.39@graphql-java.com', 'STANDARD'); </v>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (39, 'Name 39', null, 'name.39@graphql-java.com', 'STANDARD'); </v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -17765,7 +17760,7 @@
       </c>
       <c r="F41" s="5" t="str">
         <f ca="1">IF( OR(F40="commit;",F40=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('40', 'Name 40', 'Alias of Name 40', 'name.40@graphql-java.com', 'ADMIN'); </v>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (40, 'Name 40', 'Alias of Name 40', 'name.40@graphql-java.com', 'ADMIN'); </v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -17791,7 +17786,7 @@
       </c>
       <c r="F42" s="5" t="str">
         <f ca="1">IF( OR(F41="commit;",F41=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('41', 'Name 41', null, 'name.41@graphql-java.com', 'MODERATOR'); </v>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (41, 'Name 41', null, 'name.41@graphql-java.com', 'MODERATOR'); </v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -17817,7 +17812,7 @@
       </c>
       <c r="F43" s="5" t="str">
         <f ca="1">IF( OR(F42="commit;",F42=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('42', 'Name 42', 'Alias of Name 42', 'name.42@graphql-java.com', 'STANDARD'); </v>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (42, 'Name 42', 'Alias of Name 42', 'name.42@graphql-java.com', 'STANDARD'); </v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -17843,7 +17838,7 @@
       </c>
       <c r="F44" s="5" t="str">
         <f ca="1">IF( OR(F43="commit;",F43=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('43', 'Name 43', null, 'name.43@graphql-java.com', 'ADMIN'); </v>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (43, 'Name 43', null, 'name.43@graphql-java.com', 'ADMIN'); </v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -17869,7 +17864,7 @@
       </c>
       <c r="F45" s="5" t="str">
         <f ca="1">IF( OR(F44="commit;",F44=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v xml:space="preserve">insert into member (id, name, alias, email, type) values ('44', 'Name 44', 'Alias of Name 44', 'name.44@graphql-java.com', 'MODERATOR'); </v>
+        <v xml:space="preserve">insert into member (id, name, alias, email, type) values (44, 'Name 44', 'Alias of Name 44', 'name.44@graphql-java.com', 'MODERATOR'); </v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -17895,7 +17890,7 @@
       </c>
       <c r="F46" s="5" t="str">
         <f ca="1">IF( OR(F45="commit;",F45=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v>insert into board (id, name, publicly_available) values ('1', 'Board name 1', true);</v>
+        <v>insert into board (id, name, publicly_available) values (1, 'Board name 1', true);</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -17921,7 +17916,7 @@
       </c>
       <c r="F47" s="5" t="str">
         <f ca="1">IF( OR(F46="commit;",F46=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v>insert into board (id, name, publicly_available) values ('2', 'Board name 2', false);</v>
+        <v>insert into board (id, name, publicly_available) values (2, 'Board name 2', false);</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -17947,7 +17942,7 @@
       </c>
       <c r="F48" s="5" t="str">
         <f ca="1">IF( OR(F47="commit;",F47=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v>insert into board (id, name, publicly_available) values ('3', 'Board name 3', true);</v>
+        <v>insert into board (id, name, publicly_available) values (3, 'Board name 3', true);</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -17973,7 +17968,7 @@
       </c>
       <c r="F49" s="5" t="str">
         <f ca="1">IF( OR(F48="commit;",F48=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v>insert into board (id, name, publicly_available) values ('4', 'Board name 4', true);</v>
+        <v>insert into board (id, name, publicly_available) values (4, 'Board name 4', true);</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -17999,7 +17994,7 @@
       </c>
       <c r="F50" s="5" t="str">
         <f ca="1">IF( OR(F49="commit;",F49=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v>insert into board (id, name, publicly_available) values ('5', 'Board name 5', false);</v>
+        <v>insert into board (id, name, publicly_available) values (5, 'Board name 5', false);</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -18025,7 +18020,7 @@
       </c>
       <c r="F51" s="5" t="str">
         <f ca="1">IF( OR(F50="commit;",F50=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v>insert into board (id, name, publicly_available) values ('6', 'Board name 6', true);</v>
+        <v>insert into board (id, name, publicly_available) values (6, 'Board name 6', true);</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -18051,7 +18046,7 @@
       </c>
       <c r="F52" s="5" t="str">
         <f ca="1">IF( OR(F51="commit;",F51=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v>insert into board (id, name, publicly_available) values ('7', 'Board name 7', true);</v>
+        <v>insert into board (id, name, publicly_available) values (7, 'Board name 7', true);</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -18077,7 +18072,7 @@
       </c>
       <c r="F53" s="5" t="str">
         <f ca="1">IF( OR(F52="commit;",F52=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v>insert into board (id, name, publicly_available) values ('8', 'Board name 8', false);</v>
+        <v>insert into board (id, name, publicly_available) values (8, 'Board name 8', false);</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -18103,7 +18098,7 @@
       </c>
       <c r="F54" s="5" t="str">
         <f ca="1">IF( OR(F53="commit;",F53=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v>insert into board (id, name, publicly_available) values ('9', 'Board name 9', true);</v>
+        <v>insert into board (id, name, publicly_available) values (9, 'Board name 9', true);</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -18129,7 +18124,7 @@
       </c>
       <c r="F55" s="5" t="str">
         <f ca="1">IF( OR(F54="commit;",F54=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v>insert into board (id, name, publicly_available) values ('10', 'Board name 10', true);</v>
+        <v>insert into board (id, name, publicly_available) values (10, 'Board name 10', true);</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -18155,7 +18150,7 @@
       </c>
       <c r="F56" s="5" t="str">
         <f ca="1">IF( OR(F55="commit;",F55=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('1', '1', '2018-12-30 12:56:10', '1', true, 1, 'The title of &lt;1&gt;', 'The content of the topic &lt;1&gt;');</v>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (1, 1, '2018-12-30 12:56:10', 1, true, 1, 'The title of &lt;1&gt;', 'The content of the topic &lt;1&gt;');</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -18181,7 +18176,7 @@
       </c>
       <c r="F57" s="5" t="str">
         <f ca="1">IF( OR(F56="commit;",F56=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('2', '2', '2018-12-29 13:57:10', '2', true, 2, 'The title of &lt;2&gt;', 'The content of the topic &lt;2&gt;');</v>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (2, 2, '2018-12-29 13:57:10', 2, true, 2, 'The title of &lt;2&gt;', 'The content of the topic &lt;2&gt;');</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -18207,7 +18202,7 @@
       </c>
       <c r="F58" s="5" t="str">
         <f ca="1">IF( OR(F57="commit;",F57=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('3', '3', '2018-12-28 14:58:10', '3', true, 3, 'The title of &lt;3&gt;', 'The content of the topic &lt;3&gt;');</v>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (3, 3, '2018-12-28 14:58:10', 3, true, 3, 'The title of &lt;3&gt;', 'The content of the topic &lt;3&gt;');</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -18233,7 +18228,7 @@
       </c>
       <c r="F59" s="5" t="str">
         <f ca="1">IF( OR(F58="commit;",F58=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('4', '4', '2018-12-27 15:59:10', '4', true, 4, 'The title of &lt;4&gt;', 'The content of the topic &lt;4&gt;');</v>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (4, 4, '2018-12-27 15:59:10', 4, true, 4, 'The title of &lt;4&gt;', 'The content of the topic &lt;4&gt;');</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -18259,7 +18254,7 @@
       </c>
       <c r="F60" s="5" t="str">
         <f ca="1">IF( OR(F59="commit;",F59=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('5', '5', '2018-12-26 17:00:10', '5', true, 5, 'The title of &lt;5&gt;', 'The content of the topic &lt;5&gt;');</v>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (5, 5, '2018-12-26 17:00:10', 5, true, 5, 'The title of &lt;5&gt;', 'The content of the topic &lt;5&gt;');</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -18285,7 +18280,7 @@
       </c>
       <c r="F61" s="5" t="str">
         <f ca="1">IF( OR(F60="commit;",F60=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('6', '6', '2018-12-25 18:01:10', '6', true, 6, 'The title of &lt;6&gt;', 'The content of the topic &lt;6&gt;');</v>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (6, 6, '2018-12-25 18:01:10', 6, true, 6, 'The title of &lt;6&gt;', 'The content of the topic &lt;6&gt;');</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -18311,7 +18306,7 @@
       </c>
       <c r="F62" s="5" t="str">
         <f ca="1">IF( OR(F61="commit;",F61=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('7', '7', '2018-12-24 19:02:10', '7', true, 7, 'The title of &lt;7&gt;', 'The content of the topic &lt;7&gt;');</v>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (7, 7, '2018-12-24 19:02:10', 7, true, 7, 'The title of &lt;7&gt;', 'The content of the topic &lt;7&gt;');</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -18337,7 +18332,7 @@
       </c>
       <c r="F63" s="5" t="str">
         <f ca="1">IF( OR(F62="commit;",F62=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('8', '8', '2018-12-23 20:03:10', '8', true, 8, 'The title of &lt;8&gt;', 'The content of the topic &lt;8&gt;');</v>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (8, 8, '2018-12-23 20:03:10', 8, true, 8, 'The title of &lt;8&gt;', 'The content of the topic &lt;8&gt;');</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -18363,7 +18358,7 @@
       </c>
       <c r="F64" s="5" t="str">
         <f ca="1">IF( OR(F63="commit;",F63=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('9', '9', '2018-12-22 21:04:10', '9', false, 9, 'The title of &lt;9&gt;', 'The content of the topic &lt;9&gt;');</v>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (9, 9, '2018-12-22 21:04:10', 9, false, 9, 'The title of &lt;9&gt;', 'The content of the topic &lt;9&gt;');</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -18389,7 +18384,7 @@
       </c>
       <c r="F65" s="5" t="str">
         <f ca="1">IF( OR(F64="commit;",F64=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('10', '10', '2018-12-21 22:05:10', '10', true, 10, 'The title of &lt;10&gt;', 'The content of the topic &lt;10&gt;');</v>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (10, 10, '2018-12-21 22:05:10', 10, true, 10, 'The title of &lt;10&gt;', 'The content of the topic &lt;10&gt;');</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
@@ -18415,7 +18410,7 @@
       </c>
       <c r="F66" s="5" t="str">
         <f ca="1">IF( OR(F65="commit;",F65=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('11', '1', '2018-12-20 23:06:10', '11', true, 11, 'The title of &lt;11&gt;', 'The content of the topic &lt;11&gt;');</v>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (11, 1, '2018-12-20 23:06:10', 11, true, 11, 'The title of &lt;11&gt;', 'The content of the topic &lt;11&gt;');</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
@@ -18441,7 +18436,7 @@
       </c>
       <c r="F67" s="5" t="str">
         <f ca="1">IF( OR(F66="commit;",F66=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('12', '2', '2018-12-20 00:07:10', '12', true, 12, 'The title of &lt;12&gt;', 'The content of the topic &lt;12&gt;');</v>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (12, 2, '2018-12-20 00:07:10', 12, true, 12, 'The title of &lt;12&gt;', 'The content of the topic &lt;12&gt;');</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -18467,7 +18462,7 @@
       </c>
       <c r="F68" s="5" t="str">
         <f ca="1">IF( OR(F67="commit;",F67=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('13', '3', '2018-12-19 01:08:10', '13', true, 13, 'The title of &lt;13&gt;', 'The content of the topic &lt;13&gt;');</v>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (13, 3, '2018-12-19 01:08:10', 13, true, 13, 'The title of &lt;13&gt;', 'The content of the topic &lt;13&gt;');</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -18493,7 +18488,7 @@
       </c>
       <c r="F69" s="5" t="str">
         <f ca="1">IF( OR(F68="commit;",F68=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('14', '4', '2018-12-18 02:09:10', '14', true, 14, 'The title of &lt;14&gt;', 'The content of the topic &lt;14&gt;');</v>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (14, 4, '2018-12-18 02:09:10', 14, true, 14, 'The title of &lt;14&gt;', 'The content of the topic &lt;14&gt;');</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
@@ -18519,7 +18514,7 @@
       </c>
       <c r="F70" s="5" t="str">
         <f ca="1">IF( OR(F69="commit;",F69=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('15', '5', '2018-12-17 02:10:10', '15', true, 15, 'The title of &lt;15&gt;', 'The content of the topic &lt;15&gt;');</v>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (15, 5, '2018-12-17 02:10:10', 15, true, 15, 'The title of &lt;15&gt;', 'The content of the topic &lt;15&gt;');</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -18545,7 +18540,7 @@
       </c>
       <c r="F71" s="5" t="str">
         <f ca="1">IF( OR(F70="commit;",F70=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('16', '6', '2018-12-16 03:11:10', '16', true, 16, 'The title of &lt;16&gt;', 'The content of the topic &lt;16&gt;');</v>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (16, 6, '2018-12-16 03:11:10', 16, true, 16, 'The title of &lt;16&gt;', 'The content of the topic &lt;16&gt;');</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
@@ -18571,7 +18566,7 @@
       </c>
       <c r="F72" s="5" t="str">
         <f ca="1">IF( OR(F71="commit;",F71=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('17', '7', '2018-12-15 04:12:10', '17', true, 17, 'The title of &lt;17&gt;', 'The content of the topic &lt;17&gt;');</v>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (17, 7, '2018-12-15 04:12:10', 17, true, 17, 'The title of &lt;17&gt;', 'The content of the topic &lt;17&gt;');</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
@@ -18597,7 +18592,7 @@
       </c>
       <c r="F73" s="5" t="str">
         <f ca="1">IF( OR(F72="commit;",F72=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('18', '8', '2018-12-14 05:13:10', '18', true, 18, 'The title of &lt;18&gt;', 'The content of the topic &lt;18&gt;');</v>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (18, 8, '2018-12-14 05:13:10', 18, true, 18, 'The title of &lt;18&gt;', 'The content of the topic &lt;18&gt;');</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
@@ -18623,7 +18618,7 @@
       </c>
       <c r="F74" s="5" t="str">
         <f ca="1">IF( OR(F73="commit;",F73=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('19', '9', '2018-12-13 06:14:10', '19', false, 19, 'The title of &lt;19&gt;', 'The content of the topic &lt;19&gt;');</v>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (19, 9, '2018-12-13 06:14:10', 19, false, 19, 'The title of &lt;19&gt;', 'The content of the topic &lt;19&gt;');</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
@@ -18649,7 +18644,7 @@
       </c>
       <c r="F75" s="5" t="str">
         <f ca="1">IF( OR(F74="commit;",F74=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('20', '10', '2018-12-12 07:15:10', '20', true, 20, 'The title of &lt;20&gt;', 'The content of the topic &lt;20&gt;');</v>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (20, 10, '2018-12-12 07:15:10', 20, true, 20, 'The title of &lt;20&gt;', 'The content of the topic &lt;20&gt;');</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -18675,7 +18670,7 @@
       </c>
       <c r="F76" s="5" t="str">
         <f ca="1">IF( OR(F75="commit;",F75=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('21', '1', '2018-12-11 08:16:10', '21', true, 21, 'The title of &lt;21&gt;', 'The content of the topic &lt;21&gt;');</v>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (21, 1, '2018-12-11 08:16:10', 21, true, 21, 'The title of &lt;21&gt;', 'The content of the topic &lt;21&gt;');</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -18701,7 +18696,7 @@
       </c>
       <c r="F77" s="5" t="str">
         <f ca="1">IF( OR(F76="commit;",F76=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('22', '2', '2018-12-09 10:17:10', '22', true, 22, 'The title of &lt;22&gt;', 'The content of the topic &lt;22&gt;');</v>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (22, 2, '2018-12-09 10:17:10', 22, true, 22, 'The title of &lt;22&gt;', 'The content of the topic &lt;22&gt;');</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
@@ -18727,7 +18722,7 @@
       </c>
       <c r="F78" s="5" t="str">
         <f ca="1">IF( OR(F77="commit;",F77=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('23', '3', '2018-12-08 11:18:10', '23', true, 23, 'The title of &lt;23&gt;', 'The content of the topic &lt;23&gt;');</v>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (23, 3, '2018-12-08 11:18:10', 23, true, 23, 'The title of &lt;23&gt;', 'The content of the topic &lt;23&gt;');</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -18753,7 +18748,7 @@
       </c>
       <c r="F79" s="5" t="str">
         <f ca="1">IF( OR(F78="commit;",F78=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('24', '4', '2018-12-07 12:19:10', '24', true, 24, 'The title of &lt;24&gt;', 'The content of the topic &lt;24&gt;');</v>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (24, 4, '2018-12-07 12:19:10', 24, true, 24, 'The title of &lt;24&gt;', 'The content of the topic &lt;24&gt;');</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
@@ -18779,7 +18774,7 @@
       </c>
       <c r="F80" s="5" t="str">
         <f ca="1">IF( OR(F79="commit;",F79=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('25', '5', '2018-12-06 13:20:10', '25', true, 25, 'The title of &lt;25&gt;', 'The content of the topic &lt;25&gt;');</v>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (25, 5, '2018-12-06 13:20:10', 25, true, 25, 'The title of &lt;25&gt;', 'The content of the topic &lt;25&gt;');</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
@@ -18805,7 +18800,7 @@
       </c>
       <c r="F81" s="5" t="str">
         <f ca="1">IF( OR(F80="commit;",F80=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('26', '6', '2018-12-05 14:21:10', '26', true, 26, 'The title of &lt;26&gt;', 'The content of the topic &lt;26&gt;');</v>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (26, 6, '2018-12-05 14:21:10', 26, true, 26, 'The title of &lt;26&gt;', 'The content of the topic &lt;26&gt;');</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
@@ -18831,7 +18826,7 @@
       </c>
       <c r="F82" s="5" t="str">
         <f ca="1">IF( OR(F81="commit;",F81=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('27', '7', '2018-12-04 15:22:10', '27', true, 27, 'The title of &lt;27&gt;', 'The content of the topic &lt;27&gt;');</v>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (27, 7, '2018-12-04 15:22:10', 27, true, 27, 'The title of &lt;27&gt;', 'The content of the topic &lt;27&gt;');</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -18857,7 +18852,7 @@
       </c>
       <c r="F83" s="5" t="str">
         <f ca="1">IF( OR(F82="commit;",F82=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('28', '8', '2018-12-03 16:23:10', '28', true, 28, 'The title of &lt;28&gt;', 'The content of the topic &lt;28&gt;');</v>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (28, 8, '2018-12-03 16:23:10', 28, true, 28, 'The title of &lt;28&gt;', 'The content of the topic &lt;28&gt;');</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -18883,7 +18878,7 @@
       </c>
       <c r="F84" s="5" t="str">
         <f ca="1">IF( OR(F83="commit;",F83=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('29', '9', '2018-12-02 17:24:10', '29', false, 29, 'The title of &lt;29&gt;', 'The content of the topic &lt;29&gt;');</v>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (29, 9, '2018-12-02 17:24:10', 29, false, 29, 'The title of &lt;29&gt;', 'The content of the topic &lt;29&gt;');</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
@@ -18909,7 +18904,7 @@
       </c>
       <c r="F85" s="5" t="str">
         <f ca="1">IF( OR(F84="commit;",F84=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('30', '10', '2018-12-01 18:25:10', '30', true, 30, 'The title of &lt;30&gt;', 'The content of the topic &lt;30&gt;');</v>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (30, 10, '2018-12-01 18:25:10', 30, true, 30, 'The title of &lt;30&gt;', 'The content of the topic &lt;30&gt;');</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
@@ -18935,7 +18930,7 @@
       </c>
       <c r="F86" s="5" t="str">
         <f ca="1">IF( OR(F85="commit;",F85=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('31', '1', '2018-11-30 19:26:10', '31', true, 31, 'The title of &lt;31&gt;', 'The content of the topic &lt;31&gt;');</v>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (31, 1, '2018-11-30 19:26:10', 31, true, 31, 'The title of &lt;31&gt;', 'The content of the topic &lt;31&gt;');</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
@@ -18961,7 +18956,7 @@
       </c>
       <c r="F87" s="5" t="str">
         <f ca="1">IF( OR(F86="commit;",F86=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('32', '2', '2018-11-29 20:27:10', '32', true, 32, 'The title of &lt;32&gt;', 'The content of the topic &lt;32&gt;');</v>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (32, 2, '2018-11-29 20:27:10', 32, true, 32, 'The title of &lt;32&gt;', 'The content of the topic &lt;32&gt;');</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
@@ -18987,7 +18982,7 @@
       </c>
       <c r="F88" s="5" t="str">
         <f ca="1">IF( OR(F87="commit;",F87=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('33', '3', '2018-11-28 21:28:10', '33', true, 33, 'The title of &lt;33&gt;', 'The content of the topic &lt;33&gt;');</v>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (33, 3, '2018-11-28 21:28:10', 33, true, 33, 'The title of &lt;33&gt;', 'The content of the topic &lt;33&gt;');</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
@@ -19013,7 +19008,7 @@
       </c>
       <c r="F89" s="5" t="str">
         <f ca="1">IF( OR(F88="commit;",F88=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('34', '4', '2018-11-27 22:29:10', '34', true, 34, 'The title of &lt;34&gt;', 'The content of the topic &lt;34&gt;');</v>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (34, 4, '2018-11-27 22:29:10', 34, true, 34, 'The title of &lt;34&gt;', 'The content of the topic &lt;34&gt;');</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
@@ -19039,7 +19034,7 @@
       </c>
       <c r="F90" s="5" t="str">
         <f ca="1">IF( OR(F89="commit;",F89=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('35', '5', '2018-11-26 23:30:10', '35', true, 35, 'The title of &lt;35&gt;', 'The content of the topic &lt;35&gt;');</v>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (35, 5, '2018-11-26 23:30:10', 35, true, 35, 'The title of &lt;35&gt;', 'The content of the topic &lt;35&gt;');</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
@@ -19065,7 +19060,7 @@
       </c>
       <c r="F91" s="5" t="str">
         <f ca="1">IF( OR(F90="commit;",F90=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('36', '6', '2018-11-26 00:31:10', '36', true, 36, 'The title of &lt;36&gt;', 'The content of the topic &lt;36&gt;');</v>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (36, 6, '2018-11-26 00:31:10', 36, true, 36, 'The title of &lt;36&gt;', 'The content of the topic &lt;36&gt;');</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
@@ -19091,7 +19086,7 @@
       </c>
       <c r="F92" s="5" t="str">
         <f ca="1">IF( OR(F91="commit;",F91=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('37', '7', '2018-11-25 01:32:10', '37', true, 37, 'The title of &lt;37&gt;', 'The content of the topic &lt;37&gt;');</v>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (37, 7, '2018-11-25 01:32:10', 37, true, 37, 'The title of &lt;37&gt;', 'The content of the topic &lt;37&gt;');</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
@@ -19117,7 +19112,7 @@
       </c>
       <c r="F93" s="5" t="str">
         <f ca="1">IF( OR(F92="commit;",F92=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('38', '8', '2018-11-24 02:33:10', '38', true, 38, 'The title of &lt;38&gt;', 'The content of the topic &lt;38&gt;');</v>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (38, 8, '2018-11-24 02:33:10', 38, true, 38, 'The title of &lt;38&gt;', 'The content of the topic &lt;38&gt;');</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
@@ -19143,7 +19138,7 @@
       </c>
       <c r="F94" s="5" t="str">
         <f ca="1">IF( OR(F93="commit;",F93=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('39', '9', '2018-11-23 03:34:10', '39', false, 39, 'The title of &lt;39&gt;', 'The content of the topic &lt;39&gt;');</v>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (39, 9, '2018-11-23 03:34:10', 39, false, 39, 'The title of &lt;39&gt;', 'The content of the topic &lt;39&gt;');</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
@@ -19169,7 +19164,7 @@
       </c>
       <c r="F95" s="5" t="str">
         <f ca="1">IF( OR(F94="commit;",F94=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('40', '10', '2018-11-22 04:35:10', '40', true, 40, 'The title of &lt;40&gt;', 'The content of the topic &lt;40&gt;');</v>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (40, 10, '2018-11-22 04:35:10', 40, true, 40, 'The title of &lt;40&gt;', 'The content of the topic &lt;40&gt;');</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
@@ -19195,7 +19190,7 @@
       </c>
       <c r="F96" s="5" t="str">
         <f ca="1">IF( OR(F95="commit;",F95=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('41', '1', '2018-11-21 05:36:10', '41', true, 41, 'The title of &lt;41&gt;', 'The content of the topic &lt;41&gt;');</v>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (41, 1, '2018-11-21 05:36:10', 41, true, 41, 'The title of &lt;41&gt;', 'The content of the topic &lt;41&gt;');</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
@@ -19221,7 +19216,7 @@
       </c>
       <c r="F97" s="5" t="str">
         <f ca="1">IF( OR(F96="commit;",F96=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('42', '2', '2018-11-20 06:37:10', '42', true, 42, 'The title of &lt;42&gt;', 'The content of the topic &lt;42&gt;');</v>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (42, 2, '2018-11-20 06:37:10', 42, true, 42, 'The title of &lt;42&gt;', 'The content of the topic &lt;42&gt;');</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
@@ -19247,7 +19242,7 @@
       </c>
       <c r="F98" s="5" t="str">
         <f ca="1">IF( OR(F97="commit;",F97=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('43', '3', '2018-11-19 07:38:10', '43', true, 43, 'The title of &lt;43&gt;', 'The content of the topic &lt;43&gt;');</v>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (43, 3, '2018-11-19 07:38:10', 43, true, 43, 'The title of &lt;43&gt;', 'The content of the topic &lt;43&gt;');</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
@@ -19273,7 +19268,7 @@
       </c>
       <c r="F99" s="5" t="str">
         <f ca="1">IF( OR(F98="commit;",F98=""),  "",  IF(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]] = "",    "commit;",   INDIRECT(Tableau6[[#This Row],[isMember ?]]&amp;Tableau6[[#This Row],[isBoard]]&amp;Tableau6[[#This Row],[isTopic]]&amp;Tableau6[[#This Row],[isPost]])  ))</f>
-        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values ('44', '4', '2018-11-18 08:39:10', '44', true, 44, 'The title of &lt;44&gt;', 'The content of the topic &lt;44&gt;');</v>
+        <v>insert into topic (id, board_id, date, author_id, publicly_available, nb_posts, title, content) values (44, 4, '2018-11-18 08:39:10', 44, true, 44, 'The title of &lt;44&gt;', 'The content of the topic &lt;44&gt;');</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>